<commit_message>
BOM fill out: capacitors
</commit_message>
<xml_diff>
--- a/eagle/openmv2/manufacturing/OpenMV2 - BOM.xlsx
+++ b/eagle/openmv2/manufacturing/OpenMV2 - BOM.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7875"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="461">
   <si>
     <t>Part</t>
   </si>
@@ -1099,9 +1102,6 @@
     <t>USD-47571</t>
   </si>
   <si>
-    <t>USD-47571</t>
-  </si>
-  <si>
     <t>U3</t>
   </si>
   <si>
@@ -1226,23 +1226,223 @@
   </si>
   <si>
     <t>Crystals</t>
+  </si>
+  <si>
+    <t>OC_DIGIKEY</t>
+  </si>
+  <si>
+    <t>94T5091</t>
+  </si>
+  <si>
+    <t>296-16940-1-ND</t>
+  </si>
+  <si>
+    <t>TPS2115APWR</t>
+  </si>
+  <si>
+    <t>Texas Instruments</t>
+  </si>
+  <si>
+    <t>C OR CTRLR SRC SELECT 8TSSOP</t>
+  </si>
+  <si>
+    <t>CONN MICRO SD CARD PUSH-PULL R/A</t>
+  </si>
+  <si>
+    <t>Molex Inc</t>
+  </si>
+  <si>
+    <t>47571-0001</t>
+  </si>
+  <si>
+    <t>45P6234</t>
+  </si>
+  <si>
+    <t>WM9731CT-ND</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>CC0402ZRY5V7BB104</t>
+  </si>
+  <si>
+    <t>68R4688</t>
+  </si>
+  <si>
+    <t>311-1047-2-ND</t>
+  </si>
+  <si>
+    <t>CC0402ZRY5V7BB105</t>
+  </si>
+  <si>
+    <t>CC0402ZRY5V7BB106</t>
+  </si>
+  <si>
+    <t>68R4689</t>
+  </si>
+  <si>
+    <t>CC0402ZRY5V7BB107</t>
+  </si>
+  <si>
+    <t>CC0402ZRY5V7BB108</t>
+  </si>
+  <si>
+    <t>68R4690</t>
+  </si>
+  <si>
+    <t>CC0402ZRY5V7BB109</t>
+  </si>
+  <si>
+    <t>CC0402ZRY5V7BB110</t>
+  </si>
+  <si>
+    <t>T527I476M010ATE200</t>
+  </si>
+  <si>
+    <t>Kemet</t>
+  </si>
+  <si>
+    <t>39X0244</t>
+  </si>
+  <si>
+    <t>399-10532-1-ND</t>
+  </si>
+  <si>
+    <t>C1005X5R1E105K050BC</t>
+  </si>
+  <si>
+    <t>TDK Corporation</t>
+  </si>
+  <si>
+    <t>05X9838</t>
+  </si>
+  <si>
+    <t>445-9066-1-ND</t>
+  </si>
+  <si>
+    <t>AVX Corporation</t>
+  </si>
+  <si>
+    <t>F931A107KBA</t>
+  </si>
+  <si>
+    <t>478-8195-2-ND</t>
+  </si>
+  <si>
+    <t>TL8A0107M010C</t>
+  </si>
+  <si>
+    <t>Vishay Sprague</t>
+  </si>
+  <si>
+    <t>79X2068</t>
+  </si>
+  <si>
+    <t>718-1921-1-ND</t>
+  </si>
+  <si>
+    <t>C1005X5R1A475M050BC</t>
+  </si>
+  <si>
+    <t>04X3214</t>
+  </si>
+  <si>
+    <t>C1005X5R0J106M050BC</t>
+  </si>
+  <si>
+    <t>445-8920-1-ND</t>
+  </si>
+  <si>
+    <t>05X9827</t>
+  </si>
+  <si>
+    <t>GRM219R61E106KA12D</t>
+  </si>
+  <si>
+    <t>Murata Electronics North America</t>
+  </si>
+  <si>
+    <t>68X2791</t>
+  </si>
+  <si>
+    <t>490-7207-1-ND</t>
+  </si>
+  <si>
+    <t>C1005X5R1A225K050BC</t>
+  </si>
+  <si>
+    <t>445-7392-1-ND</t>
+  </si>
+  <si>
+    <t>04X3212</t>
+  </si>
+  <si>
+    <t>TPSB107M010R0400</t>
+  </si>
+  <si>
+    <t>478-5231-2-ND</t>
+  </si>
+  <si>
+    <t>10R5878</t>
+  </si>
+  <si>
+    <t>500R07S180GV4T</t>
+  </si>
+  <si>
+    <t>712-1264-1-ND</t>
+  </si>
+  <si>
+    <t>Johanson Technology Inc</t>
+  </si>
+  <si>
+    <t>41M1570</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="8">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
-    <font/>
     <font>
-      <sz val="9.0"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica neue"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1250,7 +1450,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="2">
@@ -1266,1880 +1466,2720 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
+  <cellXfs count="14">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1"/>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Hoja1"/>
+  <dimension ref="A1:Z84"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="3" customWidth="1" max="3" width="23.14"/>
-    <col min="4" customWidth="1" max="4" width="20.29"/>
-    <col min="5" customWidth="1" max="5" width="28.43"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="28.42578125" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c t="s" s="1" r="A1">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c t="s" s="1" r="B1">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c t="s" s="1" r="C1">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c t="s" s="1" r="D1">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c t="s" s="1" r="E1">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c t="s" s="1" r="F1">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c t="s" s="1" r="G1">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c t="s" s="1" r="H1">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="1" r="I1">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c s="2" r="J1"/>
-      <c s="3" r="K1"/>
-      <c s="3" r="L1"/>
-      <c s="3" r="M1"/>
-      <c s="3" r="N1"/>
-      <c s="3" r="O1"/>
-      <c s="3" r="P1"/>
-      <c s="3" r="Q1"/>
-      <c s="3" r="R1"/>
-      <c s="3" r="S1"/>
-      <c s="3" r="T1"/>
-      <c s="3" r="U1"/>
-      <c s="3" r="V1"/>
-      <c s="3" r="W1"/>
-      <c s="3" r="X1"/>
-      <c s="3" r="Y1"/>
-      <c s="3" r="Z1"/>
-    </row>
-    <row r="2">
-      <c t="s" s="4" r="A2">
+      <c r="J1" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+    </row>
+    <row r="2" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c t="s" s="4" r="B2">
+      <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c t="s" s="4" r="C2">
+      <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
-      <c t="s" s="4" r="D2">
+      <c r="D2" s="4" t="s">
         <v>12</v>
       </c>
-      <c t="s" s="4" r="E2">
+      <c r="E2" s="4" t="s">
         <v>13</v>
       </c>
-      <c s="5" r="F2"/>
-      <c s="5" r="G2"/>
-      <c s="5" r="H2"/>
-      <c s="5" r="I2"/>
-      <c s="5" r="J2"/>
-    </row>
-    <row r="3">
-      <c t="s" s="4" r="A3">
+      <c r="F2" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>416</v>
+      </c>
+      <c r="H2" s="12">
+        <v>1362417</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>417</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
-      <c t="s" s="4" r="B3">
+      <c r="B3" s="4" t="s">
         <v>15</v>
       </c>
-      <c t="s" s="4" r="C3">
+      <c r="C3" s="4" t="s">
         <v>16</v>
       </c>
-      <c t="s" s="4" r="D3">
+      <c r="D3" s="4" t="s">
         <v>17</v>
       </c>
-      <c t="s" s="4" r="E3">
+      <c r="E3" s="4" t="s">
         <v>18</v>
       </c>
-      <c s="5" r="F3"/>
-      <c s="5" r="G3"/>
-      <c s="5" r="H3"/>
-      <c s="5" r="I3"/>
-      <c s="5" r="J3"/>
-    </row>
-    <row r="4">
-      <c t="s" s="4" r="A4">
+      <c r="F3" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>416</v>
+      </c>
+      <c r="H3" s="12">
+        <v>1362417</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>417</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A4" s="4" t="s">
         <v>19</v>
       </c>
-      <c t="s" s="4" r="B4">
+      <c r="B4" s="4" t="s">
         <v>20</v>
       </c>
-      <c t="s" s="4" r="C4">
+      <c r="C4" s="4" t="s">
         <v>21</v>
       </c>
-      <c t="s" s="4" r="D4">
+      <c r="D4" s="4" t="s">
         <v>22</v>
       </c>
-      <c t="s" s="4" r="E4">
+      <c r="E4" s="4" t="s">
         <v>23</v>
       </c>
-      <c s="5" r="F4"/>
-      <c s="5" r="G4"/>
-      <c s="5" r="H4"/>
-      <c s="5" r="I4"/>
-      <c s="5" r="J4"/>
-    </row>
-    <row r="5">
-      <c t="s" s="4" r="A5">
+      <c r="F4" s="13" t="s">
+        <v>428</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="H4" s="12">
+        <v>2390053</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>429</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A5" s="4" t="s">
         <v>24</v>
       </c>
-      <c t="s" s="4" r="B5">
+      <c r="B5" s="4" t="s">
         <v>25</v>
       </c>
-      <c t="s" s="4" r="C5">
+      <c r="C5" s="4" t="s">
         <v>26</v>
       </c>
-      <c t="s" s="4" r="D5">
+      <c r="D5" s="4" t="s">
         <v>27</v>
       </c>
-      <c t="s" s="4" r="E5">
+      <c r="E5" s="4" t="s">
         <v>28</v>
       </c>
-      <c s="5" r="F5"/>
-      <c s="5" r="G5"/>
-      <c s="5" r="H5"/>
-      <c s="5" r="I5"/>
-      <c s="5" r="J5"/>
-    </row>
-    <row r="6">
-      <c t="s" s="4" r="A6">
+      <c r="F5" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>431</v>
+      </c>
+      <c r="H5" s="12">
+        <v>2346884</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>433</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A6" s="4" t="s">
         <v>29</v>
       </c>
-      <c t="s" s="4" r="B6">
+      <c r="B6" s="4" t="s">
         <v>30</v>
       </c>
-      <c t="s" s="4" r="C6">
+      <c r="C6" s="4" t="s">
         <v>31</v>
       </c>
-      <c t="s" s="4" r="D6">
+      <c r="D6" s="4" t="s">
         <v>32</v>
       </c>
-      <c t="s" s="4" r="E6">
+      <c r="E6" s="4" t="s">
         <v>33</v>
       </c>
-      <c s="5" r="F6"/>
-      <c s="5" r="G6"/>
-      <c s="5" r="H6"/>
-      <c s="5" r="I6"/>
-      <c s="5" r="J6"/>
-    </row>
-    <row r="7">
-      <c t="s" s="4" r="A7">
+      <c r="F6" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>416</v>
+      </c>
+      <c r="H6" s="12">
+        <v>1362417</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>417</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A7" s="4" t="s">
         <v>34</v>
       </c>
-      <c t="s" s="4" r="B7">
+      <c r="B7" s="4" t="s">
         <v>35</v>
       </c>
-      <c t="s" s="4" r="C7">
+      <c r="C7" s="4" t="s">
         <v>36</v>
       </c>
-      <c t="s" s="4" r="D7">
+      <c r="D7" s="4" t="s">
         <v>37</v>
       </c>
-      <c t="s" s="4" r="E7">
+      <c r="E7" s="4" t="s">
         <v>38</v>
       </c>
-      <c s="5" r="F7"/>
-      <c s="5" r="G7"/>
-      <c s="5" r="H7"/>
-      <c s="5" r="I7"/>
-      <c s="5" r="J7"/>
-    </row>
-    <row r="8">
-      <c t="s" s="4" r="A8">
+      <c r="F7" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>416</v>
+      </c>
+      <c r="H7" s="12">
+        <v>1362417</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>417</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A8" s="4" t="s">
         <v>39</v>
       </c>
-      <c t="s" s="4" r="B8">
+      <c r="B8" s="4" t="s">
         <v>40</v>
       </c>
-      <c t="s" s="4" r="C8">
+      <c r="C8" s="4" t="s">
         <v>41</v>
       </c>
-      <c t="s" s="4" r="D8">
+      <c r="D8" s="4" t="s">
         <v>42</v>
       </c>
-      <c t="s" s="4" r="E8">
+      <c r="E8" s="4" t="s">
         <v>43</v>
       </c>
-      <c s="5" r="F8"/>
-      <c s="5" r="G8"/>
-      <c s="5" r="H8"/>
-      <c s="5" r="I8"/>
-      <c s="5" r="J8"/>
-    </row>
-    <row r="9">
-      <c t="s" s="4" r="A9">
+      <c r="F8" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>419</v>
+      </c>
+      <c r="H8" s="12">
+        <v>1362417</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>417</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A9" s="4" t="s">
         <v>44</v>
       </c>
-      <c t="s" s="4" r="B9">
+      <c r="B9" s="4" t="s">
         <v>45</v>
       </c>
-      <c t="s" s="4" r="C9">
+      <c r="C9" s="4" t="s">
         <v>46</v>
       </c>
-      <c t="s" s="4" r="D9">
+      <c r="D9" s="4" t="s">
         <v>47</v>
       </c>
-      <c t="s" s="4" r="E9">
+      <c r="E9" s="4" t="s">
         <v>48</v>
       </c>
-      <c s="5" r="F9"/>
-      <c s="5" r="G9"/>
-      <c s="5" r="H9"/>
-      <c s="5" r="I9"/>
-      <c s="5" r="J9"/>
-    </row>
-    <row r="10">
-      <c t="s" s="4" r="A10">
+      <c r="F9" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="H9" s="12">
+        <v>1362417</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>417</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A10" s="4" t="s">
         <v>49</v>
       </c>
-      <c t="s" s="4" r="B10">
+      <c r="B10" s="4" t="s">
         <v>50</v>
       </c>
-      <c t="s" s="4" r="C10">
+      <c r="C10" s="4" t="s">
         <v>51</v>
       </c>
-      <c t="s" s="4" r="D10">
+      <c r="D10" s="4" t="s">
         <v>52</v>
       </c>
-      <c t="s" s="4" r="E10">
+      <c r="E10" s="4" t="s">
         <v>53</v>
       </c>
-      <c s="5" r="F10"/>
-      <c s="5" r="G10"/>
-      <c s="5" r="H10"/>
-      <c s="5" r="I10"/>
-      <c s="5" r="J10"/>
-    </row>
-    <row r="11">
-      <c t="s" s="4" r="A11">
+      <c r="F10" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="H10" s="12">
+        <v>1362417</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>421</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A11" s="4" t="s">
         <v>54</v>
       </c>
-      <c t="s" s="4" r="B11">
+      <c r="B11" s="4" t="s">
         <v>55</v>
       </c>
-      <c t="s" s="4" r="C11">
+      <c r="C11" s="4" t="s">
         <v>56</v>
       </c>
-      <c t="s" s="4" r="D11">
+      <c r="D11" s="4" t="s">
         <v>57</v>
       </c>
-      <c t="s" s="4" r="E11">
+      <c r="E11" s="4" t="s">
         <v>58</v>
       </c>
-      <c s="5" r="F11"/>
-      <c s="5" r="G11"/>
-      <c s="5" r="H11"/>
-      <c s="5" r="I11"/>
-      <c s="5" r="J11"/>
-    </row>
-    <row r="12">
-      <c t="s" s="4" r="A12">
+      <c r="F11" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>423</v>
+      </c>
+      <c r="H11" s="12">
+        <v>1362417</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A12" s="4" t="s">
         <v>59</v>
       </c>
-      <c t="s" s="4" r="B12">
+      <c r="B12" s="4" t="s">
         <v>60</v>
       </c>
-      <c t="s" s="4" r="C12">
+      <c r="C12" s="4" t="s">
         <v>61</v>
       </c>
-      <c t="s" s="4" r="D12">
+      <c r="D12" s="4" t="s">
         <v>62</v>
       </c>
-      <c t="s" s="4" r="E12">
+      <c r="E12" s="4" t="s">
         <v>63</v>
       </c>
-      <c s="5" r="F12"/>
-      <c s="5" r="G12"/>
-      <c s="5" r="H12"/>
-      <c s="5" r="I12"/>
-      <c s="5" r="J12"/>
-    </row>
-    <row r="13">
-      <c t="s" s="4" r="A13">
+      <c r="F12" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>436</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="12" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A13" s="4" t="s">
         <v>64</v>
       </c>
-      <c t="s" s="4" r="B13">
+      <c r="B13" s="4" t="s">
         <v>65</v>
       </c>
-      <c t="s" s="4" r="C13">
+      <c r="C13" s="4" t="s">
         <v>66</v>
       </c>
-      <c t="s" s="4" r="D13">
+      <c r="D13" s="4" t="s">
         <v>67</v>
       </c>
-      <c t="s" s="4" r="E13">
+      <c r="E13" s="4" t="s">
         <v>68</v>
       </c>
-      <c s="5" r="F13"/>
-      <c s="5" r="G13"/>
-      <c s="5" r="H13"/>
-      <c s="5" r="I13"/>
-      <c s="5" r="J13"/>
-    </row>
-    <row r="14">
-      <c t="s" s="4" r="A14">
+      <c r="F13" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="H13" s="12">
+        <v>2425585</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A14" s="13" t="s">
         <v>69</v>
       </c>
-      <c t="s" s="4" r="B14">
+      <c r="B14" s="4" t="s">
         <v>70</v>
       </c>
-      <c t="s" s="4" r="C14">
+      <c r="C14" s="4" t="s">
         <v>71</v>
       </c>
-      <c t="s" s="4" r="D14">
+      <c r="D14" s="4" t="s">
         <v>72</v>
       </c>
-      <c t="s" s="4" r="E14">
+      <c r="E14" s="4" t="s">
         <v>73</v>
       </c>
-      <c s="5" r="F14"/>
-      <c s="5" r="G14"/>
-      <c s="5" r="H14"/>
-      <c s="5" r="I14"/>
-      <c s="5" r="J14"/>
-    </row>
-    <row r="15">
-      <c t="s" s="4" r="A15">
+      <c r="F14" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>423</v>
+      </c>
+      <c r="H14" s="12">
+        <v>1362417</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A15" s="4" t="s">
         <v>74</v>
       </c>
-      <c t="s" s="4" r="B15">
+      <c r="B15" s="4" t="s">
         <v>75</v>
       </c>
-      <c t="s" s="4" r="C15">
+      <c r="C15" s="4" t="s">
         <v>76</v>
       </c>
-      <c t="s" s="4" r="D15">
+      <c r="D15" s="4" t="s">
         <v>77</v>
       </c>
-      <c t="s" s="4" r="E15">
+      <c r="E15" s="4" t="s">
         <v>78</v>
       </c>
-      <c s="5" r="F15"/>
-      <c s="5" r="G15"/>
-      <c s="5" r="H15"/>
-      <c s="5" r="I15"/>
-      <c s="5" r="J15"/>
-    </row>
-    <row r="16">
-      <c t="s" s="4" r="A16">
+      <c r="F15" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>425</v>
+      </c>
+      <c r="H15" s="12">
+        <v>1362417</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A16" s="13" t="s">
         <v>79</v>
       </c>
-      <c t="s" s="4" r="B16">
+      <c r="B16" s="4" t="s">
         <v>80</v>
       </c>
-      <c t="s" s="4" r="C16">
+      <c r="C16" s="4" t="s">
         <v>81</v>
       </c>
-      <c t="s" s="4" r="D16">
+      <c r="D16" s="4" t="s">
         <v>82</v>
       </c>
-      <c t="s" s="4" r="E16">
+      <c r="E16" s="4" t="s">
         <v>83</v>
       </c>
-      <c s="5" r="F16"/>
-      <c s="5" r="G16"/>
-      <c s="5" r="H16"/>
-      <c s="5" r="I16"/>
-      <c s="5" r="J16"/>
-    </row>
-    <row r="17">
-      <c t="s" s="4" r="A17">
+      <c r="F16" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>442</v>
+      </c>
+      <c r="H16" s="12">
+        <v>2346881</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A17" s="4" t="s">
         <v>84</v>
       </c>
-      <c t="s" s="4" r="B17">
+      <c r="B17" s="4" t="s">
         <v>85</v>
       </c>
-      <c t="s" s="4" r="C17">
+      <c r="C17" s="4" t="s">
         <v>86</v>
       </c>
-      <c t="s" s="4" r="D17">
+      <c r="D17" s="4" t="s">
         <v>87</v>
       </c>
-      <c t="s" s="4" r="E17">
+      <c r="E17" s="4" t="s">
         <v>88</v>
       </c>
-      <c s="5" r="F17"/>
-      <c s="5" r="G17"/>
-      <c s="5" r="H17"/>
-      <c s="5" r="I17"/>
-      <c s="5" r="J17"/>
-    </row>
-    <row r="18">
-      <c t="s" s="4" r="A18">
+      <c r="F17" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>425</v>
+      </c>
+      <c r="H17" s="12">
+        <v>1362417</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A18" s="4" t="s">
         <v>89</v>
       </c>
-      <c t="s" s="4" r="B18">
+      <c r="B18" s="4" t="s">
         <v>90</v>
       </c>
-      <c t="s" s="4" r="C18">
+      <c r="C18" s="4" t="s">
         <v>91</v>
       </c>
-      <c t="s" s="4" r="D18">
+      <c r="D18" s="4" t="s">
         <v>92</v>
       </c>
-      <c t="s" s="4" r="E18">
+      <c r="E18" s="4" t="s">
         <v>93</v>
       </c>
-      <c s="5" r="F18"/>
-      <c s="5" r="G18"/>
-      <c s="5" r="H18"/>
-      <c s="5" r="I18"/>
-      <c s="5" r="J18"/>
-    </row>
-    <row r="19">
-      <c t="s" s="4" r="A19">
+      <c r="F18" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>426</v>
+      </c>
+      <c r="H18" s="12">
+        <v>1362417</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A19" s="4" t="s">
         <v>94</v>
       </c>
-      <c t="s" s="4" r="B19">
+      <c r="B19" s="4" t="s">
         <v>95</v>
       </c>
-      <c t="s" s="4" r="C19">
+      <c r="C19" s="4" t="s">
         <v>96</v>
       </c>
-      <c t="s" s="4" r="D19">
+      <c r="D19" s="4" t="s">
         <v>97</v>
       </c>
-      <c t="s" s="4" r="E19">
+      <c r="E19" s="4" t="s">
         <v>98</v>
       </c>
-      <c s="5" r="F19"/>
-      <c s="5" r="G19"/>
-      <c s="5" r="H19"/>
-      <c s="5" r="I19"/>
-      <c s="5" r="J19"/>
-    </row>
-    <row r="20">
-      <c t="s" s="4" r="A20">
+      <c r="F19" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>426</v>
+      </c>
+      <c r="H19" s="12">
+        <v>1362417</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="J19" s="12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A20" s="4" t="s">
         <v>99</v>
       </c>
-      <c t="s" s="4" r="B20">
+      <c r="B20" s="4" t="s">
         <v>100</v>
       </c>
-      <c t="s" s="4" r="C20">
+      <c r="C20" s="4" t="s">
         <v>101</v>
       </c>
-      <c t="s" s="4" r="D20">
+      <c r="D20" s="4" t="s">
         <v>102</v>
       </c>
-      <c t="s" s="4" r="E20">
+      <c r="E20" s="4" t="s">
         <v>103</v>
       </c>
-      <c s="5" r="F20"/>
-      <c s="5" r="G20"/>
-      <c s="5" r="H20"/>
-      <c s="5" r="I20"/>
-      <c s="5" r="J20"/>
-    </row>
-    <row r="21">
-      <c t="s" s="4" r="A21">
+      <c r="F20" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>442</v>
+      </c>
+      <c r="H20" s="12">
+        <v>2346881</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A21" s="4" t="s">
         <v>104</v>
       </c>
-      <c t="s" s="4" r="B21">
+      <c r="B21" s="4" t="s">
         <v>105</v>
       </c>
-      <c t="s" s="4" r="C21">
+      <c r="C21" s="4" t="s">
         <v>106</v>
       </c>
-      <c t="s" s="4" r="D21">
+      <c r="D21" s="4" t="s">
         <v>107</v>
       </c>
-      <c t="s" s="4" r="E21">
+      <c r="E21" s="4" t="s">
         <v>108</v>
       </c>
-      <c s="5" r="F21"/>
-      <c s="5" r="G21"/>
-      <c s="5" r="H21"/>
-      <c s="5" r="I21"/>
-      <c s="5" r="J21"/>
-    </row>
-    <row r="22">
-      <c t="s" s="4" r="A22">
+      <c r="F21" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>426</v>
+      </c>
+      <c r="H21" s="12">
+        <v>1362417</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A22" s="4" t="s">
         <v>109</v>
       </c>
-      <c t="s" s="4" r="B22">
+      <c r="B22" s="4" t="s">
         <v>110</v>
       </c>
-      <c t="s" s="4" r="C22">
+      <c r="C22" s="4" t="s">
         <v>111</v>
       </c>
-      <c t="s" s="4" r="D22">
+      <c r="D22" s="4" t="s">
         <v>112</v>
       </c>
-      <c t="s" s="4" r="E22">
+      <c r="E22" s="4" t="s">
         <v>113</v>
       </c>
-      <c s="5" r="F22"/>
-      <c s="5" r="G22"/>
-      <c s="5" r="H22"/>
-      <c s="5" r="I22"/>
-      <c s="5" r="J22"/>
-    </row>
-    <row r="23">
-      <c t="s" s="4" r="A23">
+      <c r="F22" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="H22" s="12">
+        <v>2425585</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="J22" s="12" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A23" s="4" t="s">
         <v>114</v>
       </c>
-      <c t="s" s="4" r="B23">
+      <c r="B23" s="4" t="s">
         <v>115</v>
       </c>
-      <c t="s" s="4" r="C23">
+      <c r="C23" s="4" t="s">
         <v>116</v>
       </c>
-      <c t="s" s="4" r="D23">
+      <c r="D23" s="4" t="s">
         <v>117</v>
       </c>
-      <c t="s" s="4" r="E23">
+      <c r="E23" s="4" t="s">
         <v>118</v>
       </c>
-      <c s="5" r="F23"/>
-      <c s="5" r="G23"/>
-      <c s="5" r="H23"/>
-      <c s="5" r="I23"/>
-      <c s="5" r="J23"/>
-    </row>
-    <row r="24">
-      <c t="s" s="4" r="A24">
+      <c r="F23" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="H23" s="12">
+        <v>2346872</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>446</v>
+      </c>
+      <c r="J23" s="12" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A24" s="4" t="s">
         <v>119</v>
       </c>
-      <c t="s" s="4" r="B24">
+      <c r="B24" s="4" t="s">
         <v>120</v>
       </c>
-      <c t="s" s="4" r="C24">
+      <c r="C24" s="4" t="s">
         <v>121</v>
       </c>
-      <c t="s" s="4" r="D24">
+      <c r="D24" s="4" t="s">
         <v>122</v>
       </c>
-      <c t="s" s="4" r="E24">
+      <c r="E24" s="4" t="s">
         <v>123</v>
       </c>
-      <c s="5" r="F24"/>
-      <c s="5" r="G24"/>
-      <c s="5" r="H24"/>
-      <c s="5" r="I24"/>
-      <c s="5" r="J24"/>
-    </row>
-    <row r="25">
-      <c t="s" s="4" r="A25">
+      <c r="F24" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>444</v>
+      </c>
+      <c r="H24" s="12">
+        <v>2346872</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>446</v>
+      </c>
+      <c r="J24" s="12" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A25" s="4" t="s">
         <v>124</v>
       </c>
-      <c t="s" s="4" r="B25">
+      <c r="B25" s="4" t="s">
         <v>125</v>
       </c>
-      <c t="s" s="4" r="C25">
+      <c r="C25" s="4" t="s">
         <v>126</v>
       </c>
-      <c t="s" s="4" r="D25">
+      <c r="D25" s="4" t="s">
         <v>127</v>
       </c>
-      <c t="s" s="4" r="E25">
+      <c r="E25" s="4" t="s">
         <v>128</v>
       </c>
-      <c s="5" r="F25"/>
-      <c s="5" r="G25"/>
-      <c s="5" r="H25"/>
-      <c s="5" r="I25"/>
-      <c s="5" r="J25"/>
-    </row>
-    <row r="26">
-      <c t="s" s="4" r="A26">
+      <c r="F25" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>426</v>
+      </c>
+      <c r="H25" s="12">
+        <v>1362417</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="J25" s="12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A26" s="4" t="s">
         <v>129</v>
       </c>
-      <c t="s" s="4" r="B26">
+      <c r="B26" s="4" t="s">
         <v>130</v>
       </c>
-      <c t="s" s="4" r="C26">
+      <c r="C26" s="4" t="s">
         <v>131</v>
       </c>
-      <c t="s" s="4" r="D26">
+      <c r="D26" s="4" t="s">
         <v>132</v>
       </c>
-      <c t="s" s="4" r="E26">
+      <c r="E26" s="4" t="s">
         <v>133</v>
       </c>
-      <c s="5" r="F26"/>
-      <c s="5" r="G26"/>
-      <c s="5" r="H26"/>
-      <c s="5" r="I26"/>
-      <c s="5" r="J26"/>
-    </row>
-    <row r="27">
-      <c t="s" s="4" r="A27">
+      <c r="F26" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>426</v>
+      </c>
+      <c r="H26" s="12">
+        <v>1362417</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="J26" s="12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A27" s="4" t="s">
         <v>134</v>
       </c>
-      <c t="s" s="4" r="B27">
+      <c r="B27" s="4" t="s">
         <v>135</v>
       </c>
-      <c t="s" s="4" r="C27">
+      <c r="C27" s="4" t="s">
         <v>136</v>
       </c>
-      <c t="s" s="4" r="D27">
+      <c r="D27" s="4" t="s">
         <v>137</v>
       </c>
-      <c t="s" s="4" r="E27">
+      <c r="E27" s="4" t="s">
         <v>138</v>
       </c>
-      <c s="5" r="F27"/>
-      <c s="5" r="G27"/>
-      <c s="5" r="H27"/>
-      <c s="5" r="I27"/>
-      <c s="5" r="J27"/>
-    </row>
-    <row r="28">
-      <c t="s" s="4" r="A28">
+      <c r="F27" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>426</v>
+      </c>
+      <c r="H27" s="12">
+        <v>1362417</v>
+      </c>
+      <c r="I27" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="J27" s="12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A28" s="4" t="s">
         <v>139</v>
       </c>
-      <c t="s" s="4" r="B28">
+      <c r="B28" s="4" t="s">
         <v>140</v>
       </c>
-      <c t="s" s="4" r="C28">
+      <c r="C28" s="4" t="s">
         <v>141</v>
       </c>
-      <c t="s" s="4" r="D28">
+      <c r="D28" s="4" t="s">
         <v>142</v>
       </c>
-      <c t="s" s="4" r="E28">
+      <c r="E28" s="4" t="s">
         <v>143</v>
       </c>
-      <c s="5" r="F28"/>
-      <c s="5" r="G28"/>
-      <c s="5" r="H28"/>
-      <c s="5" r="I28"/>
-      <c s="5" r="J28"/>
-    </row>
-    <row r="29">
-      <c t="s" s="4" r="A29">
+      <c r="F28" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>426</v>
+      </c>
+      <c r="H28" s="12">
+        <v>1362417</v>
+      </c>
+      <c r="I28" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="J28" s="12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A29" s="4" t="s">
         <v>144</v>
       </c>
-      <c t="s" s="4" r="B29">
+      <c r="B29" s="4" t="s">
         <v>145</v>
       </c>
-      <c t="s" s="4" r="C29">
+      <c r="C29" s="4" t="s">
         <v>146</v>
       </c>
-      <c t="s" s="4" r="D29">
+      <c r="D29" s="4" t="s">
         <v>147</v>
       </c>
-      <c t="s" s="4" r="E29">
+      <c r="E29" s="4" t="s">
         <v>148</v>
       </c>
-      <c s="5" r="F29"/>
-      <c s="5" r="G29"/>
-      <c s="5" r="H29"/>
-      <c s="5" r="I29"/>
-      <c s="5" r="J29"/>
-    </row>
-    <row r="30">
-      <c t="s" s="4" r="A30">
+      <c r="F29" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>426</v>
+      </c>
+      <c r="H29" s="12">
+        <v>1362417</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="J29" s="12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A30" s="4" t="s">
         <v>149</v>
       </c>
-      <c t="s" s="4" r="B30">
+      <c r="B30" s="4" t="s">
         <v>150</v>
       </c>
-      <c t="s" s="4" r="C30">
+      <c r="C30" s="4" t="s">
         <v>151</v>
       </c>
-      <c s="4" r="D30">
-        <v>805.0</v>
-      </c>
-      <c t="s" s="4" r="E30">
+      <c r="D30" s="4">
+        <v>805</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>152</v>
       </c>
-      <c s="5" r="F30"/>
-      <c s="5" r="G30"/>
-      <c s="5" r="H30"/>
-      <c s="5" r="I30"/>
-      <c s="5" r="J30"/>
-    </row>
-    <row r="31">
-      <c t="s" s="4" r="A31">
+      <c r="F30" s="8" t="s">
+        <v>448</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>447</v>
+      </c>
+      <c r="H30" s="12">
+        <v>2426961</v>
+      </c>
+      <c r="I30" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="J30" s="12" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A31" s="4" t="s">
         <v>153</v>
       </c>
-      <c t="s" s="4" r="B31">
+      <c r="B31" s="4" t="s">
         <v>154</v>
       </c>
-      <c t="s" s="4" r="C31">
+      <c r="C31" s="4" t="s">
         <v>155</v>
       </c>
-      <c t="s" s="4" r="D31">
+      <c r="D31" s="4" t="s">
         <v>156</v>
       </c>
-      <c t="s" s="4" r="E31">
+      <c r="E31" s="4" t="s">
         <v>157</v>
       </c>
-      <c s="5" r="F31"/>
-      <c s="5" r="G31"/>
-      <c s="5" r="H31"/>
-      <c s="5" r="I31"/>
-      <c s="5" r="J31"/>
-    </row>
-    <row r="32">
-      <c t="s" s="4" r="A32">
+      <c r="F31" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>426</v>
+      </c>
+      <c r="H31" s="12">
+        <v>1362417</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="J31" s="12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A32" s="4" t="s">
         <v>158</v>
       </c>
-      <c t="s" s="4" r="B32">
+      <c r="B32" s="4" t="s">
         <v>159</v>
       </c>
-      <c t="s" s="4" r="C32">
+      <c r="C32" s="4" t="s">
         <v>160</v>
       </c>
-      <c t="s" s="4" r="D32">
+      <c r="D32" s="4" t="s">
         <v>161</v>
       </c>
-      <c t="s" s="4" r="E32">
+      <c r="E32" s="4" t="s">
         <v>162</v>
       </c>
-      <c s="5" r="F32"/>
-      <c s="5" r="G32"/>
-      <c s="5" r="H32"/>
-      <c s="5" r="I32"/>
-      <c s="5" r="J32"/>
-    </row>
-    <row r="33">
-      <c t="s" s="4" r="A33">
+      <c r="F32" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>426</v>
+      </c>
+      <c r="H32" s="12">
+        <v>1362417</v>
+      </c>
+      <c r="I32" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="J32" s="12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A33" s="4" t="s">
         <v>163</v>
       </c>
-      <c t="s" s="4" r="B33">
+      <c r="B33" s="4" t="s">
         <v>164</v>
       </c>
-      <c t="s" s="4" r="C33">
+      <c r="C33" s="4" t="s">
         <v>165</v>
       </c>
-      <c t="s" s="4" r="D33">
+      <c r="D33" s="4" t="s">
         <v>166</v>
       </c>
-      <c t="s" s="4" r="E33">
+      <c r="E33" s="4" t="s">
         <v>167</v>
       </c>
-      <c s="5" r="F33"/>
-      <c s="5" r="G33"/>
-      <c s="5" r="H33"/>
-      <c s="5" r="I33"/>
-      <c s="5" r="J33"/>
-    </row>
-    <row r="34">
-      <c t="s" s="4" r="A34">
+      <c r="F33" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="H33" s="12">
+        <v>2346879</v>
+      </c>
+      <c r="I33" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="J33" s="12" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A34" s="4" t="s">
         <v>168</v>
       </c>
-      <c t="s" s="4" r="B34">
+      <c r="B34" s="4" t="s">
         <v>169</v>
       </c>
-      <c t="s" s="4" r="C34">
+      <c r="C34" s="4" t="s">
         <v>170</v>
       </c>
-      <c t="s" s="4" r="D34">
+      <c r="D34" s="4" t="s">
         <v>171</v>
       </c>
-      <c t="s" s="4" r="E34">
+      <c r="E34" s="4" t="s">
         <v>172</v>
       </c>
-      <c s="5" r="F34"/>
-      <c s="5" r="G34"/>
-      <c s="5" r="H34"/>
-      <c s="5" r="I34"/>
-      <c s="5" r="J34"/>
-    </row>
-    <row r="35">
-      <c t="s" s="4" r="A35">
+      <c r="F34" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="H34" s="12">
+        <v>2346879</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="J34" s="12" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A35" s="4" t="s">
         <v>173</v>
       </c>
-      <c t="s" s="4" r="B35">
+      <c r="B35" s="4" t="s">
         <v>174</v>
       </c>
-      <c t="s" s="4" r="C35">
+      <c r="C35" s="4" t="s">
         <v>175</v>
       </c>
-      <c t="s" s="4" r="D35">
+      <c r="D35" s="4" t="s">
         <v>176</v>
       </c>
-      <c t="s" s="4" r="E35">
+      <c r="E35" s="4" t="s">
         <v>177</v>
       </c>
-      <c s="5" r="F35"/>
-      <c s="5" r="G35"/>
-      <c s="5" r="H35"/>
-      <c s="5" r="I35"/>
-      <c s="5" r="J35"/>
-    </row>
-    <row r="36">
-      <c t="s" s="4" r="A36">
+      <c r="F35" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>426</v>
+      </c>
+      <c r="H35" s="12">
+        <v>1362417</v>
+      </c>
+      <c r="I35" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="J35" s="12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A36" s="4" t="s">
         <v>178</v>
       </c>
-      <c t="s" s="4" r="B36">
+      <c r="B36" s="4" t="s">
         <v>179</v>
       </c>
-      <c t="s" s="4" r="C36">
+      <c r="C36" s="4" t="s">
         <v>180</v>
       </c>
-      <c t="s" s="4" r="D36">
+      <c r="D36" s="4" t="s">
         <v>181</v>
       </c>
-      <c t="s" s="4" r="E36">
+      <c r="E36" s="4" t="s">
         <v>182</v>
       </c>
-      <c s="5" r="F36"/>
-      <c s="5" r="G36"/>
-      <c s="5" r="H36"/>
-      <c s="5" r="I36"/>
-      <c s="5" r="J36"/>
-    </row>
-    <row r="37">
-      <c t="s" s="4" r="A37">
+      <c r="F36" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>426</v>
+      </c>
+      <c r="H36" s="12">
+        <v>1362417</v>
+      </c>
+      <c r="I36" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="J36" s="12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A37" s="4" t="s">
         <v>183</v>
       </c>
-      <c t="s" s="4" r="B37">
+      <c r="B37" s="4" t="s">
         <v>184</v>
       </c>
-      <c t="s" s="4" r="C37">
+      <c r="C37" s="4" t="s">
         <v>185</v>
       </c>
-      <c t="s" s="4" r="D37">
+      <c r="D37" s="4" t="s">
         <v>186</v>
       </c>
-      <c t="s" s="4" r="E37">
+      <c r="E37" s="4" t="s">
         <v>187</v>
       </c>
-      <c s="5" r="F37"/>
-      <c s="5" r="G37"/>
-      <c s="5" r="H37"/>
-      <c s="5" r="I37"/>
-      <c s="5" r="J37"/>
-    </row>
-    <row r="38">
-      <c t="s" s="4" r="A38">
+      <c r="F37" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>426</v>
+      </c>
+      <c r="H37" s="12">
+        <v>1362417</v>
+      </c>
+      <c r="I37" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="J37" s="12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A38" s="4" t="s">
         <v>188</v>
       </c>
-      <c t="s" s="4" r="B38">
+      <c r="B38" s="4" t="s">
         <v>189</v>
       </c>
-      <c t="s" s="4" r="C38">
+      <c r="C38" s="4" t="s">
         <v>190</v>
       </c>
-      <c t="s" s="4" r="D38">
+      <c r="D38" s="4" t="s">
         <v>191</v>
       </c>
-      <c t="s" s="4" r="E38">
+      <c r="E38" s="4" t="s">
         <v>192</v>
       </c>
-      <c s="5" r="F38"/>
-      <c s="5" r="G38"/>
-      <c s="5" r="H38"/>
-      <c s="5" r="I38"/>
-      <c s="5" r="J38"/>
-    </row>
-    <row r="39">
-      <c t="s" s="4" r="A39">
+      <c r="F38" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>454</v>
+      </c>
+      <c r="H38" s="12">
+        <v>1658510</v>
+      </c>
+      <c r="I38" s="12" t="s">
+        <v>456</v>
+      </c>
+      <c r="J38" s="12" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A39" s="4" t="s">
         <v>193</v>
       </c>
-      <c t="s" s="4" r="B39">
+      <c r="B39" s="4" t="s">
         <v>194</v>
       </c>
-      <c t="s" s="4" r="C39">
+      <c r="C39" s="4" t="s">
         <v>195</v>
       </c>
-      <c t="s" s="4" r="D39">
+      <c r="D39" s="4" t="s">
         <v>196</v>
       </c>
-      <c t="s" s="4" r="E39">
+      <c r="E39" s="4" t="s">
         <v>197</v>
       </c>
-      <c s="5" r="F39"/>
-      <c s="5" r="G39"/>
-      <c s="5" r="H39"/>
-      <c s="5" r="I39"/>
-      <c s="5" r="J39"/>
-    </row>
-    <row r="40">
-      <c t="s" s="4" r="A40">
+      <c r="F39" s="8" t="s">
+        <v>459</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>457</v>
+      </c>
+      <c r="H39" s="12">
+        <v>1650783</v>
+      </c>
+      <c r="I39" s="12" t="s">
+        <v>460</v>
+      </c>
+      <c r="J39" s="12" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A40" s="4" t="s">
         <v>198</v>
       </c>
-      <c t="s" s="4" r="B40">
+      <c r="B40" s="4" t="s">
         <v>199</v>
       </c>
-      <c t="s" s="4" r="C40">
+      <c r="C40" s="4" t="s">
         <v>200</v>
       </c>
-      <c t="s" s="4" r="D40">
+      <c r="D40" s="4" t="s">
         <v>201</v>
       </c>
-      <c t="s" s="4" r="E40">
+      <c r="E40" s="4" t="s">
         <v>202</v>
       </c>
-      <c s="5" r="F40"/>
-      <c s="5" r="G40"/>
-      <c s="5" r="H40"/>
-      <c s="5" r="I40"/>
-      <c s="5" r="J40"/>
-    </row>
-    <row r="41">
-      <c t="s" s="4" r="A41">
+      <c r="F40" s="8" t="s">
+        <v>459</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>457</v>
+      </c>
+      <c r="H40" s="12">
+        <v>1650783</v>
+      </c>
+      <c r="I40" s="12" t="s">
+        <v>460</v>
+      </c>
+      <c r="J40" s="12" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A41" s="4" t="s">
         <v>203</v>
       </c>
-      <c t="s" s="4" r="B41">
+      <c r="B41" s="4" t="s">
         <v>204</v>
       </c>
-      <c t="s" s="4" r="C41">
+      <c r="C41" s="4" t="s">
         <v>205</v>
       </c>
-      <c t="s" s="4" r="D41">
+      <c r="D41" s="4" t="s">
         <v>206</v>
       </c>
-      <c t="s" s="4" r="E41">
+      <c r="E41" s="4" t="s">
         <v>207</v>
       </c>
-      <c s="5" r="F41"/>
-      <c s="5" r="G41"/>
-      <c s="5" r="H41"/>
-      <c s="5" r="I41"/>
-      <c s="5" r="J41"/>
-    </row>
-    <row r="42">
-      <c t="s" s="4" r="A42">
+      <c r="F41" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="G41" s="10" t="s">
+        <v>426</v>
+      </c>
+      <c r="H41" s="12">
+        <v>1362417</v>
+      </c>
+      <c r="I41" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="J41" s="12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A42" s="4" t="s">
         <v>208</v>
       </c>
-      <c t="s" s="4" r="B42">
+      <c r="B42" s="4" t="s">
         <v>209</v>
       </c>
-      <c t="s" s="4" r="C42">
+      <c r="C42" s="4" t="s">
         <v>210</v>
       </c>
-      <c t="s" s="4" r="D42">
+      <c r="D42" s="4" t="s">
         <v>211</v>
       </c>
-      <c t="s" s="4" r="E42">
+      <c r="E42" s="4" t="s">
         <v>212</v>
       </c>
-      <c s="5" r="F42"/>
-      <c s="5" r="G42"/>
-      <c s="5" r="H42"/>
-      <c s="5" r="I42"/>
-      <c s="5" r="J42"/>
-    </row>
-    <row r="43">
-      <c t="s" s="4" r="A43">
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+    </row>
+    <row r="43" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A43" s="4" t="s">
         <v>213</v>
       </c>
-      <c t="s" s="4" r="B43">
+      <c r="B43" s="4" t="s">
         <v>214</v>
       </c>
-      <c t="s" s="4" r="C43">
+      <c r="C43" s="4" t="s">
         <v>215</v>
       </c>
-      <c t="s" s="4" r="D43">
+      <c r="D43" s="4" t="s">
         <v>216</v>
       </c>
-      <c t="s" s="4" r="E43">
+      <c r="E43" s="4" t="s">
         <v>217</v>
       </c>
-      <c s="5" r="F43"/>
-      <c s="5" r="G43"/>
-      <c s="5" r="H43"/>
-      <c s="5" r="I43"/>
-      <c s="5" r="J43"/>
-    </row>
-    <row r="44">
-      <c t="s" s="4" r="A44">
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+    </row>
+    <row r="44" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A44" s="4" t="s">
         <v>218</v>
       </c>
-      <c t="s" s="4" r="B44">
+      <c r="B44" s="4" t="s">
         <v>219</v>
       </c>
-      <c t="s" s="4" r="C44">
+      <c r="C44" s="4" t="s">
         <v>220</v>
       </c>
-      <c t="s" s="4" r="D44">
+      <c r="D44" s="4" t="s">
         <v>221</v>
       </c>
-      <c t="s" s="4" r="E44">
+      <c r="E44" s="4" t="s">
         <v>222</v>
       </c>
-      <c s="5" r="F44"/>
-      <c s="5" r="G44"/>
-      <c s="5" r="H44"/>
-      <c s="5" r="I44"/>
-      <c s="5" r="J44"/>
-    </row>
-    <row r="45">
-      <c t="s" s="4" r="A45">
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+    </row>
+    <row r="45" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A45" s="4" t="s">
         <v>223</v>
       </c>
-      <c t="s" s="4" r="B45">
+      <c r="B45" s="4" t="s">
         <v>224</v>
       </c>
-      <c t="s" s="4" r="C45">
+      <c r="C45" s="4" t="s">
         <v>225</v>
       </c>
-      <c t="s" s="4" r="D45">
+      <c r="D45" s="4" t="s">
         <v>226</v>
       </c>
-      <c t="s" s="4" r="E45">
+      <c r="E45" s="4" t="s">
         <v>227</v>
       </c>
-      <c s="5" r="F45"/>
-      <c s="5" r="G45"/>
-      <c s="5" r="H45"/>
-      <c s="5" r="I45"/>
-      <c s="5" r="J45"/>
-    </row>
-    <row r="46">
-      <c t="s" s="4" r="A46">
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+    </row>
+    <row r="46" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A46" s="4" t="s">
         <v>228</v>
       </c>
-      <c t="s" s="4" r="B46">
+      <c r="B46" s="4" t="s">
         <v>229</v>
       </c>
-      <c t="s" s="4" r="C46">
+      <c r="C46" s="4" t="s">
         <v>230</v>
       </c>
-      <c t="s" s="4" r="D46">
+      <c r="D46" s="4" t="s">
         <v>231</v>
       </c>
-      <c s="5" r="E46"/>
-      <c s="5" r="F46"/>
-      <c s="5" r="G46"/>
-      <c s="5" r="H46"/>
-      <c s="5" r="I46"/>
-      <c s="5" r="J46"/>
-    </row>
-    <row r="47">
-      <c t="s" s="4" r="A47">
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+    </row>
+    <row r="47" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A47" s="4" t="s">
         <v>232</v>
       </c>
-      <c t="s" s="4" r="B47">
+      <c r="B47" s="4" t="s">
         <v>233</v>
       </c>
-      <c t="s" s="4" r="C47">
+      <c r="C47" s="4" t="s">
         <v>234</v>
       </c>
-      <c t="s" s="4" r="D47">
+      <c r="D47" s="4" t="s">
         <v>235</v>
       </c>
-      <c s="5" r="E47"/>
-      <c s="5" r="F47"/>
-      <c s="5" r="G47"/>
-      <c s="5" r="H47"/>
-      <c s="5" r="I47"/>
-      <c s="5" r="J47"/>
-    </row>
-    <row r="48">
-      <c t="s" s="4" r="A48">
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+    </row>
+    <row r="48" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A48" s="4" t="s">
         <v>236</v>
       </c>
-      <c s="5" r="B48"/>
-      <c t="s" s="4" r="C48">
+      <c r="B48" s="5"/>
+      <c r="C48" s="4" t="s">
         <v>237</v>
       </c>
-      <c t="s" s="4" r="D48">
+      <c r="D48" s="4" t="s">
         <v>238</v>
       </c>
-      <c t="s" s="4" r="E48">
+      <c r="E48" s="4" t="s">
         <v>239</v>
       </c>
-      <c s="5" r="F48"/>
-      <c s="5" r="G48"/>
-      <c s="5" r="H48"/>
-      <c s="5" r="I48"/>
-      <c s="5" r="J48"/>
-    </row>
-    <row r="49">
-      <c t="s" s="4" r="A49">
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+    </row>
+    <row r="49" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A49" s="4" t="s">
         <v>240</v>
       </c>
-      <c s="5" r="B49"/>
-      <c t="s" s="4" r="C49">
+      <c r="B49" s="5"/>
+      <c r="C49" s="4" t="s">
         <v>241</v>
       </c>
-      <c t="s" s="4" r="D49">
+      <c r="D49" s="4" t="s">
         <v>242</v>
       </c>
-      <c t="s" s="4" r="E49">
+      <c r="E49" s="4" t="s">
         <v>243</v>
       </c>
-      <c s="5" r="F49"/>
-      <c s="5" r="G49"/>
-      <c s="5" r="H49"/>
-      <c s="5" r="I49"/>
-      <c s="5" r="J49"/>
-    </row>
-    <row r="50">
-      <c t="s" s="4" r="A50">
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+    </row>
+    <row r="50" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A50" s="4" t="s">
         <v>244</v>
       </c>
-      <c t="s" s="4" r="B50">
+      <c r="B50" s="4" t="s">
         <v>245</v>
       </c>
-      <c t="s" s="4" r="C50">
+      <c r="C50" s="4" t="s">
         <v>246</v>
       </c>
-      <c t="s" s="4" r="D50">
+      <c r="D50" s="4" t="s">
         <v>247</v>
       </c>
-      <c t="s" s="4" r="E50">
+      <c r="E50" s="4" t="s">
         <v>248</v>
       </c>
-      <c s="5" r="F50"/>
-      <c s="5" r="G50"/>
-      <c s="5" r="H50"/>
-      <c s="5" r="I50"/>
-      <c s="5" r="J50"/>
-    </row>
-    <row r="51">
-      <c t="s" s="4" r="A51">
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+    </row>
+    <row r="51" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A51" s="4" t="s">
         <v>249</v>
       </c>
-      <c s="5" r="B51"/>
-      <c t="s" s="4" r="C51">
+      <c r="B51" s="5"/>
+      <c r="C51" s="4" t="s">
         <v>250</v>
       </c>
-      <c t="s" s="4" r="D51">
+      <c r="D51" s="4" t="s">
         <v>251</v>
       </c>
-      <c t="s" s="4" r="E51">
+      <c r="E51" s="4" t="s">
         <v>252</v>
       </c>
-      <c s="5" r="F51"/>
-      <c s="5" r="G51"/>
-      <c s="5" r="H51"/>
-      <c s="5" r="I51"/>
-      <c s="5" r="J51"/>
-    </row>
-    <row r="52">
-      <c t="s" s="4" r="A52">
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+    </row>
+    <row r="52" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A52" s="4" t="s">
         <v>253</v>
       </c>
-      <c s="5" r="B52"/>
-      <c t="s" s="4" r="C52">
+      <c r="B52" s="5"/>
+      <c r="C52" s="4" t="s">
         <v>254</v>
       </c>
-      <c t="s" s="4" r="D52">
+      <c r="D52" s="4" t="s">
         <v>255</v>
       </c>
-      <c t="s" s="4" r="E52">
+      <c r="E52" s="4" t="s">
         <v>256</v>
       </c>
-      <c s="5" r="F52"/>
-      <c s="5" r="G52"/>
-      <c s="5" r="H52"/>
-      <c s="5" r="I52"/>
-      <c s="5" r="J52"/>
-    </row>
-    <row r="53">
-      <c t="s" s="4" r="A53">
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5"/>
+      <c r="J52" s="5"/>
+    </row>
+    <row r="53" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A53" s="4" t="s">
         <v>257</v>
       </c>
-      <c t="s" s="4" r="B53">
+      <c r="B53" s="4" t="s">
         <v>258</v>
       </c>
-      <c t="s" s="4" r="C53">
+      <c r="C53" s="4" t="s">
         <v>259</v>
       </c>
-      <c t="s" s="4" r="D53">
+      <c r="D53" s="4" t="s">
         <v>260</v>
       </c>
-      <c s="5" r="E53"/>
-      <c s="5" r="F53"/>
-      <c s="5" r="G53"/>
-      <c s="5" r="H53"/>
-      <c s="5" r="I53"/>
-      <c s="5" r="J53"/>
-    </row>
-    <row r="54">
-      <c t="s" s="4" r="A54">
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
+    </row>
+    <row r="54" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A54" s="4" t="s">
         <v>261</v>
       </c>
-      <c t="s" s="4" r="B54">
+      <c r="B54" s="4" t="s">
         <v>262</v>
       </c>
-      <c t="s" s="4" r="C54">
+      <c r="C54" s="4" t="s">
         <v>263</v>
       </c>
-      <c t="s" s="4" r="D54">
+      <c r="D54" s="4" t="s">
         <v>264</v>
       </c>
-      <c s="5" r="E54"/>
-      <c s="5" r="F54"/>
-      <c s="5" r="G54"/>
-      <c s="5" r="H54"/>
-      <c s="5" r="I54"/>
-      <c s="5" r="J54"/>
-    </row>
-    <row r="55">
-      <c t="s" s="4" r="A55">
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
+    </row>
+    <row r="55" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A55" s="4" t="s">
         <v>265</v>
       </c>
-      <c t="s" s="4" r="B55">
+      <c r="B55" s="4" t="s">
         <v>266</v>
       </c>
-      <c t="s" s="4" r="C55">
+      <c r="C55" s="4" t="s">
         <v>267</v>
       </c>
-      <c t="s" s="4" r="D55">
+      <c r="D55" s="4" t="s">
         <v>268</v>
       </c>
-      <c t="s" s="4" r="E55">
+      <c r="E55" s="4" t="s">
         <v>269</v>
       </c>
-      <c s="5" r="F55"/>
-      <c s="5" r="G55"/>
-      <c s="5" r="H55"/>
-      <c s="5" r="I55"/>
-      <c s="5" r="J55"/>
-    </row>
-    <row r="56">
-      <c t="s" s="4" r="A56">
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
+    </row>
+    <row r="56" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A56" s="4" t="s">
         <v>270</v>
       </c>
-      <c t="s" s="4" r="B56">
+      <c r="B56" s="4" t="s">
         <v>271</v>
       </c>
-      <c t="s" s="4" r="C56">
+      <c r="C56" s="4" t="s">
         <v>272</v>
       </c>
-      <c t="s" s="4" r="D56">
+      <c r="D56" s="4" t="s">
         <v>273</v>
       </c>
-      <c t="s" s="4" r="E56">
+      <c r="E56" s="4" t="s">
         <v>274</v>
       </c>
-      <c s="5" r="F56"/>
-      <c s="5" r="G56"/>
-      <c s="5" r="H56"/>
-      <c s="5" r="I56"/>
-      <c s="5" r="J56"/>
-    </row>
-    <row r="57">
-      <c t="s" s="4" r="A57">
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5"/>
+      <c r="J56" s="5"/>
+    </row>
+    <row r="57" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A57" s="4" t="s">
         <v>275</v>
       </c>
-      <c t="s" s="4" r="B57">
+      <c r="B57" s="4" t="s">
         <v>276</v>
       </c>
-      <c t="s" s="4" r="C57">
+      <c r="C57" s="4" t="s">
         <v>277</v>
       </c>
-      <c t="s" s="4" r="D57">
+      <c r="D57" s="4" t="s">
         <v>278</v>
       </c>
-      <c t="s" s="4" r="E57">
+      <c r="E57" s="4" t="s">
         <v>279</v>
       </c>
-      <c s="5" r="F57"/>
-      <c s="5" r="G57"/>
-      <c s="5" r="H57"/>
-      <c s="5" r="I57"/>
-      <c s="5" r="J57"/>
-    </row>
-    <row r="58">
-      <c t="s" s="4" r="A58">
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="5"/>
+      <c r="J57" s="5"/>
+    </row>
+    <row r="58" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A58" s="4" t="s">
         <v>280</v>
       </c>
-      <c t="s" s="4" r="B58">
+      <c r="B58" s="4" t="s">
         <v>281</v>
       </c>
-      <c t="s" s="4" r="C58">
+      <c r="C58" s="4" t="s">
         <v>282</v>
       </c>
-      <c t="s" s="4" r="D58">
+      <c r="D58" s="4" t="s">
         <v>283</v>
       </c>
-      <c t="s" s="4" r="E58">
+      <c r="E58" s="4" t="s">
         <v>284</v>
       </c>
-      <c s="5" r="F58"/>
-      <c s="5" r="G58"/>
-      <c s="5" r="H58"/>
-      <c s="5" r="I58"/>
-      <c s="5" r="J58"/>
-    </row>
-    <row r="59">
-      <c t="s" s="4" r="A59">
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+      <c r="I58" s="5"/>
+      <c r="J58" s="5"/>
+    </row>
+    <row r="59" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A59" s="4" t="s">
         <v>285</v>
       </c>
-      <c s="5" r="B59"/>
-      <c t="s" s="4" r="C59">
+      <c r="B59" s="5"/>
+      <c r="C59" s="4" t="s">
         <v>286</v>
       </c>
-      <c t="s" s="4" r="D59">
+      <c r="D59" s="4" t="s">
         <v>287</v>
       </c>
-      <c t="s" s="4" r="E59">
+      <c r="E59" s="4" t="s">
         <v>288</v>
       </c>
-      <c s="5" r="F59"/>
-      <c s="5" r="G59"/>
-      <c t="s" s="4" r="H59">
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="4" t="s">
         <v>289</v>
       </c>
-      <c t="s" s="4" r="I59">
+      <c r="I59" s="4" t="s">
         <v>290</v>
       </c>
-      <c s="5" r="J59"/>
-    </row>
-    <row r="60">
-      <c t="s" s="4" r="A60">
+      <c r="J59" s="5"/>
+    </row>
+    <row r="60" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A60" s="4" t="s">
         <v>291</v>
       </c>
-      <c s="5" r="B60"/>
-      <c t="s" s="4" r="C60">
+      <c r="B60" s="5"/>
+      <c r="C60" s="4" t="s">
         <v>292</v>
       </c>
-      <c t="s" s="4" r="D60">
+      <c r="D60" s="4" t="s">
         <v>293</v>
       </c>
-      <c t="s" s="4" r="E60">
+      <c r="E60" s="4" t="s">
         <v>294</v>
       </c>
-      <c s="5" r="F60"/>
-      <c s="5" r="G60"/>
-      <c t="s" s="4" r="H60">
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="4" t="s">
         <v>295</v>
       </c>
-      <c t="s" s="4" r="I60">
+      <c r="I60" s="4" t="s">
         <v>296</v>
       </c>
-      <c s="5" r="J60"/>
-    </row>
-    <row r="61">
-      <c t="s" s="4" r="A61">
+      <c r="J60" s="5"/>
+    </row>
+    <row r="61" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A61" s="4" t="s">
         <v>297</v>
       </c>
-      <c s="5" r="B61"/>
-      <c t="s" s="4" r="C61">
+      <c r="B61" s="5"/>
+      <c r="C61" s="4" t="s">
         <v>298</v>
       </c>
-      <c t="s" s="4" r="D61">
+      <c r="D61" s="4" t="s">
         <v>299</v>
       </c>
-      <c t="s" s="4" r="E61">
+      <c r="E61" s="4" t="s">
         <v>300</v>
       </c>
-      <c s="5" r="F61"/>
-      <c s="5" r="G61"/>
-      <c t="s" s="4" r="H61">
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="4" t="s">
         <v>301</v>
       </c>
-      <c t="s" s="4" r="I61">
+      <c r="I61" s="4" t="s">
         <v>302</v>
       </c>
-      <c s="5" r="J61"/>
-    </row>
-    <row r="62">
-      <c t="s" s="4" r="A62">
+      <c r="J61" s="5"/>
+    </row>
+    <row r="62" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A62" s="4" t="s">
         <v>303</v>
       </c>
-      <c s="5" r="B62"/>
-      <c t="s" s="4" r="C62">
+      <c r="B62" s="5"/>
+      <c r="C62" s="4" t="s">
         <v>304</v>
       </c>
-      <c t="s" s="4" r="D62">
+      <c r="D62" s="4" t="s">
         <v>305</v>
       </c>
-      <c t="s" s="4" r="E62">
+      <c r="E62" s="4" t="s">
         <v>306</v>
       </c>
-      <c s="5" r="F62"/>
-      <c s="5" r="G62"/>
-      <c t="s" s="4" r="H62">
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="4" t="s">
         <v>307</v>
       </c>
-      <c t="s" s="4" r="I62">
+      <c r="I62" s="4" t="s">
         <v>308</v>
       </c>
-      <c s="5" r="J62"/>
-    </row>
-    <row r="63">
-      <c t="s" s="4" r="A63">
+      <c r="J62" s="5"/>
+    </row>
+    <row r="63" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A63" s="4" t="s">
         <v>309</v>
       </c>
-      <c s="5" r="B63"/>
-      <c t="s" s="4" r="C63">
+      <c r="B63" s="5"/>
+      <c r="C63" s="4" t="s">
         <v>310</v>
       </c>
-      <c t="s" s="4" r="D63">
+      <c r="D63" s="4" t="s">
         <v>311</v>
       </c>
-      <c t="s" s="4" r="E63">
+      <c r="E63" s="4" t="s">
         <v>312</v>
       </c>
-      <c s="5" r="F63"/>
-      <c s="5" r="G63"/>
-      <c t="s" s="4" r="H63">
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="4" t="s">
         <v>313</v>
       </c>
-      <c t="s" s="4" r="I63">
+      <c r="I63" s="4" t="s">
         <v>314</v>
       </c>
-      <c s="5" r="J63"/>
-    </row>
-    <row r="64">
-      <c t="s" s="4" r="A64">
+      <c r="J63" s="5"/>
+    </row>
+    <row r="64" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A64" s="4" t="s">
         <v>315</v>
       </c>
-      <c s="5" r="B64"/>
-      <c t="s" s="4" r="C64">
+      <c r="B64" s="5"/>
+      <c r="C64" s="4" t="s">
         <v>316</v>
       </c>
-      <c t="s" s="4" r="D64">
+      <c r="D64" s="4" t="s">
         <v>317</v>
       </c>
-      <c t="s" s="4" r="E64">
+      <c r="E64" s="4" t="s">
         <v>318</v>
       </c>
-      <c s="5" r="F64"/>
-      <c s="5" r="G64"/>
-      <c t="s" s="4" r="H64">
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="4" t="s">
         <v>319</v>
       </c>
-      <c t="s" s="4" r="I64">
+      <c r="I64" s="4" t="s">
         <v>320</v>
       </c>
-      <c s="5" r="J64"/>
-    </row>
-    <row r="65">
-      <c t="s" s="4" r="A65">
+      <c r="J64" s="5"/>
+    </row>
+    <row r="65" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A65" s="4" t="s">
         <v>321</v>
       </c>
-      <c t="s" s="4" r="B65">
+      <c r="B65" s="4" t="s">
         <v>322</v>
       </c>
-      <c t="s" s="4" r="C65">
+      <c r="C65" s="4" t="s">
         <v>323</v>
       </c>
-      <c t="s" s="4" r="D65">
+      <c r="D65" s="4" t="s">
         <v>324</v>
       </c>
-      <c s="5" r="E65"/>
-      <c s="5" r="F65"/>
-      <c s="5" r="G65"/>
-      <c s="5" r="H65"/>
-      <c s="5" r="I65"/>
-      <c s="5" r="J65"/>
-    </row>
-    <row r="66">
-      <c t="s" s="4" r="A66">
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="5"/>
+      <c r="I65" s="5"/>
+      <c r="J65" s="5"/>
+    </row>
+    <row r="66" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A66" s="4" t="s">
         <v>325</v>
       </c>
-      <c t="s" s="4" r="B66">
+      <c r="B66" s="4" t="s">
         <v>326</v>
       </c>
-      <c t="s" s="4" r="C66">
+      <c r="C66" s="4" t="s">
         <v>327</v>
       </c>
-      <c t="s" s="4" r="D66">
+      <c r="D66" s="4" t="s">
         <v>328</v>
       </c>
-      <c t="s" s="4" r="E66">
+      <c r="E66" s="4" t="s">
         <v>329</v>
       </c>
-      <c s="5" r="F66"/>
-      <c s="5" r="G66"/>
-      <c s="5" r="H66"/>
-      <c s="5" r="I66"/>
-      <c s="5" r="J66"/>
-    </row>
-    <row r="67">
-      <c t="s" s="4" r="A67">
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+      <c r="I66" s="5"/>
+      <c r="J66" s="5"/>
+    </row>
+    <row r="67" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A67" s="4" t="s">
         <v>330</v>
       </c>
-      <c t="s" s="4" r="B67">
+      <c r="B67" s="4" t="s">
         <v>331</v>
       </c>
-      <c t="s" s="4" r="C67">
+      <c r="C67" s="4" t="s">
         <v>332</v>
       </c>
-      <c t="s" s="4" r="D67">
+      <c r="D67" s="4" t="s">
         <v>333</v>
       </c>
-      <c t="s" s="4" r="E67">
+      <c r="E67" s="4" t="s">
         <v>334</v>
       </c>
-      <c s="5" r="F67"/>
-      <c s="5" r="G67"/>
-      <c s="5" r="H67"/>
-      <c s="5" r="I67"/>
-      <c s="5" r="J67"/>
-    </row>
-    <row r="68">
-      <c t="s" s="4" r="A68">
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="5"/>
+      <c r="I67" s="5"/>
+      <c r="J67" s="5"/>
+    </row>
+    <row r="68" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A68" s="4" t="s">
         <v>335</v>
       </c>
-      <c t="s" s="4" r="B68">
+      <c r="B68" s="4" t="s">
         <v>336</v>
       </c>
-      <c t="s" s="4" r="C68">
+      <c r="C68" s="4" t="s">
         <v>337</v>
       </c>
-      <c t="s" s="4" r="D68">
+      <c r="D68" s="4" t="s">
         <v>338</v>
       </c>
-      <c t="s" s="4" r="E68">
+      <c r="E68" s="4" t="s">
         <v>339</v>
       </c>
-      <c s="5" r="F68"/>
-      <c s="5" r="G68"/>
-      <c s="5" r="H68"/>
-      <c s="5" r="I68"/>
-      <c s="5" r="J68"/>
-    </row>
-    <row r="69">
-      <c t="s" s="4" r="A69">
+      <c r="F68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5"/>
+      <c r="I68" s="5"/>
+      <c r="J68" s="5"/>
+    </row>
+    <row r="69" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A69" s="4" t="s">
         <v>340</v>
       </c>
-      <c t="s" s="4" r="B69">
+      <c r="B69" s="4" t="s">
         <v>341</v>
       </c>
-      <c t="s" s="4" r="C69">
+      <c r="C69" s="4" t="s">
         <v>342</v>
       </c>
-      <c t="s" s="4" r="D69">
+      <c r="D69" s="4" t="s">
         <v>343</v>
       </c>
-      <c t="s" s="4" r="E69">
+      <c r="E69" s="4" t="s">
         <v>344</v>
       </c>
-      <c s="5" r="F69"/>
-      <c s="5" r="G69"/>
-      <c s="5" r="H69"/>
-      <c s="5" r="I69"/>
-      <c s="5" r="J69"/>
-    </row>
-    <row r="70">
-      <c t="s" s="4" r="A70">
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="5"/>
+      <c r="I69" s="5"/>
+      <c r="J69" s="5"/>
+    </row>
+    <row r="70" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A70" s="4" t="s">
         <v>345</v>
       </c>
-      <c t="s" s="4" r="B70">
+      <c r="B70" s="4" t="s">
         <v>346</v>
       </c>
-      <c t="s" s="4" r="C70">
+      <c r="C70" s="4" t="s">
         <v>347</v>
       </c>
-      <c t="s" s="4" r="D70">
+      <c r="D70" s="4" t="s">
         <v>348</v>
       </c>
-      <c t="s" s="4" r="E70">
+      <c r="E70" s="4" t="s">
         <v>349</v>
       </c>
-      <c s="5" r="F70"/>
-      <c s="5" r="G70"/>
-      <c s="5" r="H70"/>
-      <c s="5" r="I70"/>
-      <c s="5" r="J70"/>
-    </row>
-    <row r="71">
-      <c t="s" s="4" r="A71">
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
+      <c r="J70" s="5"/>
+    </row>
+    <row r="71" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A71" s="4" t="s">
         <v>350</v>
       </c>
-      <c t="s" s="4" r="B71">
+      <c r="B71" s="4" t="s">
         <v>351</v>
       </c>
-      <c t="s" s="4" r="C71">
+      <c r="C71" s="4" t="s">
         <v>352</v>
       </c>
-      <c t="s" s="4" r="D71">
+      <c r="D71" s="4" t="s">
         <v>353</v>
       </c>
-      <c t="s" s="4" r="E71">
+      <c r="E71" s="4" t="s">
         <v>354</v>
       </c>
-      <c s="5" r="F71"/>
-      <c s="5" r="G71"/>
-      <c s="5" r="H71"/>
-      <c s="5" r="I71"/>
-      <c s="5" r="J71"/>
-    </row>
-    <row r="72">
-      <c t="s" s="4" r="A72">
+      <c r="F71" s="5"/>
+      <c r="G71" s="5"/>
+      <c r="H71" s="5"/>
+      <c r="I71" s="5"/>
+      <c r="J71" s="5"/>
+    </row>
+    <row r="72" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A72" s="4" t="s">
         <v>355</v>
       </c>
-      <c t="s" s="4" r="B72">
+      <c r="B72" s="4" t="s">
         <v>356</v>
       </c>
-      <c t="s" s="4" r="C72">
+      <c r="C72" s="4" t="s">
         <v>357</v>
       </c>
-      <c t="s" s="4" r="D72">
+      <c r="D72" s="4" t="s">
         <v>358</v>
       </c>
-      <c s="5" r="E72"/>
-      <c s="5" r="F72"/>
-      <c s="5" r="G72"/>
-      <c s="5" r="H72"/>
-      <c s="5" r="I72"/>
-      <c s="5" r="J72"/>
-    </row>
-    <row r="73">
-      <c t="s" s="4" r="A73">
+      <c r="E72" t="s">
+        <v>409</v>
+      </c>
+      <c r="F72" s="9" t="s">
+        <v>408</v>
+      </c>
+      <c r="G72" s="8" t="s">
+        <v>407</v>
+      </c>
+      <c r="H72" s="7">
+        <v>2368258</v>
+      </c>
+      <c r="I72" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="J72" s="7" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A73" s="4" t="s">
         <v>359</v>
       </c>
-      <c t="s" s="4" r="B73">
+      <c r="B73" s="4" t="s">
         <v>360</v>
       </c>
-      <c t="s" s="4" r="C73">
+      <c r="C73" s="4" t="s">
         <v>361</v>
       </c>
-      <c t="s" s="4" r="D73">
+      <c r="D73" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="E73" t="s">
+        <v>410</v>
+      </c>
+      <c r="F73" t="s">
+        <v>411</v>
+      </c>
+      <c r="G73" s="8" t="s">
+        <v>412</v>
+      </c>
+      <c r="H73" s="5"/>
+      <c r="I73" t="s">
+        <v>413</v>
+      </c>
+      <c r="J73" s="7" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A74" s="4" t="s">
         <v>362</v>
       </c>
-      <c s="5" r="E73"/>
-      <c s="5" r="F73"/>
-      <c s="5" r="G73"/>
-      <c s="5" r="H73"/>
-      <c s="5" r="I73"/>
-      <c s="5" r="J73"/>
-    </row>
-    <row r="74">
-      <c t="s" s="4" r="A74">
+      <c r="B74" s="4" t="s">
         <v>363</v>
       </c>
-      <c t="s" s="4" r="B74">
+      <c r="C74" s="4" t="s">
         <v>364</v>
       </c>
-      <c t="s" s="4" r="C74">
+      <c r="D74" s="4" t="s">
         <v>365</v>
       </c>
-      <c t="s" s="4" r="D74">
+      <c r="E74" s="5"/>
+      <c r="F74" s="5"/>
+      <c r="G74" s="5"/>
+      <c r="H74" s="5"/>
+      <c r="I74" s="5"/>
+      <c r="J74" s="5"/>
+    </row>
+    <row r="75" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A75" s="4" t="s">
         <v>366</v>
       </c>
-      <c s="5" r="E74"/>
-      <c s="5" r="F74"/>
-      <c s="5" r="G74"/>
-      <c s="5" r="H74"/>
-      <c s="5" r="I74"/>
-      <c s="5" r="J74"/>
-    </row>
-    <row r="75">
-      <c t="s" s="4" r="A75">
+      <c r="B75" s="4" t="s">
         <v>367</v>
       </c>
-      <c t="s" s="4" r="B75">
+      <c r="C75" s="4" t="s">
         <v>368</v>
       </c>
-      <c t="s" s="4" r="C75">
+      <c r="D75" s="4" t="s">
         <v>369</v>
       </c>
-      <c t="s" s="4" r="D75">
+      <c r="E75" s="5"/>
+      <c r="F75" s="5"/>
+      <c r="G75" s="5"/>
+      <c r="H75" s="5"/>
+      <c r="I75" s="5"/>
+      <c r="J75" s="5"/>
+    </row>
+    <row r="76" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A76" s="4" t="s">
         <v>370</v>
       </c>
-      <c s="5" r="E75"/>
-      <c s="5" r="F75"/>
-      <c s="5" r="G75"/>
-      <c s="5" r="H75"/>
-      <c s="5" r="I75"/>
-      <c s="5" r="J75"/>
-    </row>
-    <row r="76">
-      <c t="s" s="4" r="A76">
+      <c r="B76" s="4" t="s">
         <v>371</v>
       </c>
-      <c t="s" s="4" r="B76">
+      <c r="C76" s="4" t="s">
         <v>372</v>
       </c>
-      <c t="s" s="4" r="C76">
+      <c r="D76" s="4" t="s">
         <v>373</v>
       </c>
-      <c t="s" s="4" r="D76">
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
+      <c r="G76" s="5"/>
+      <c r="H76" s="5"/>
+      <c r="I76" s="5"/>
+      <c r="J76" s="5"/>
+    </row>
+    <row r="77" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A77" s="4" t="s">
         <v>374</v>
       </c>
-      <c s="5" r="E76"/>
-      <c s="5" r="F76"/>
-      <c s="5" r="G76"/>
-      <c s="5" r="H76"/>
-      <c s="5" r="I76"/>
-      <c s="5" r="J76"/>
-    </row>
-    <row r="77">
-      <c t="s" s="4" r="A77">
+      <c r="B77" s="4" t="s">
         <v>375</v>
       </c>
-      <c t="s" s="4" r="B77">
+      <c r="C77" s="4" t="s">
         <v>376</v>
       </c>
-      <c t="s" s="4" r="C77">
+      <c r="D77" s="4" t="s">
         <v>377</v>
       </c>
-      <c t="s" s="4" r="D77">
+      <c r="E77" s="5"/>
+      <c r="F77" s="5"/>
+      <c r="G77" s="5"/>
+      <c r="H77" s="5"/>
+      <c r="I77" s="5"/>
+      <c r="J77" s="5"/>
+    </row>
+    <row r="78" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A78" s="4" t="s">
         <v>378</v>
       </c>
-      <c s="5" r="E77"/>
-      <c s="5" r="F77"/>
-      <c s="5" r="G77"/>
-      <c s="5" r="H77"/>
-      <c s="5" r="I77"/>
-      <c s="5" r="J77"/>
-    </row>
-    <row r="78">
-      <c t="s" s="4" r="A78">
+      <c r="B78" s="4" t="s">
         <v>379</v>
       </c>
-      <c t="s" s="4" r="B78">
+      <c r="C78" s="4" t="s">
         <v>380</v>
       </c>
-      <c t="s" s="4" r="C78">
+      <c r="D78" s="4" t="s">
         <v>381</v>
       </c>
-      <c t="s" s="4" r="D78">
+      <c r="E78" s="5"/>
+      <c r="F78" s="5"/>
+      <c r="G78" s="5"/>
+      <c r="H78" s="5"/>
+      <c r="I78" s="5"/>
+      <c r="J78" s="5"/>
+    </row>
+    <row r="79" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A79" s="4" t="s">
         <v>382</v>
       </c>
-      <c s="5" r="E78"/>
-      <c s="5" r="F78"/>
-      <c s="5" r="G78"/>
-      <c s="5" r="H78"/>
-      <c s="5" r="I78"/>
-      <c s="5" r="J78"/>
-    </row>
-    <row r="79">
-      <c t="s" s="4" r="A79">
+      <c r="B79" s="4" t="s">
         <v>383</v>
       </c>
-      <c t="s" s="4" r="B79">
+      <c r="C79" s="4" t="s">
         <v>384</v>
       </c>
-      <c t="s" s="4" r="C79">
+      <c r="D79" s="4" t="s">
         <v>385</v>
       </c>
-      <c t="s" s="4" r="D79">
+      <c r="E79" s="4" t="s">
         <v>386</v>
       </c>
-      <c t="s" s="4" r="E79">
+      <c r="F79" s="5"/>
+      <c r="G79" s="5"/>
+      <c r="H79" s="5"/>
+      <c r="I79" s="5"/>
+      <c r="J79" s="5"/>
+    </row>
+    <row r="80" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A80" s="4" t="s">
         <v>387</v>
       </c>
-      <c s="5" r="F79"/>
-      <c s="5" r="G79"/>
-      <c s="5" r="H79"/>
-      <c s="5" r="I79"/>
-      <c s="5" r="J79"/>
-    </row>
-    <row r="80">
-      <c t="s" s="4" r="A80">
+      <c r="B80" s="4" t="s">
         <v>388</v>
       </c>
-      <c t="s" s="4" r="B80">
+      <c r="C80" s="4" t="s">
         <v>389</v>
       </c>
-      <c t="s" s="4" r="C80">
+      <c r="D80" s="4" t="s">
         <v>390</v>
       </c>
-      <c t="s" s="4" r="D80">
+      <c r="E80" s="5"/>
+      <c r="F80" s="5"/>
+      <c r="G80" s="5"/>
+      <c r="H80" s="5"/>
+      <c r="I80" s="5"/>
+      <c r="J80" s="5"/>
+    </row>
+    <row r="81" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A81" s="4" t="s">
         <v>391</v>
       </c>
-      <c s="5" r="E80"/>
-      <c s="5" r="F80"/>
-      <c s="5" r="G80"/>
-      <c s="5" r="H80"/>
-      <c s="5" r="I80"/>
-      <c s="5" r="J80"/>
-    </row>
-    <row r="81">
-      <c t="s" s="4" r="A81">
+      <c r="B81" s="4" t="s">
         <v>392</v>
       </c>
-      <c t="s" s="4" r="B81">
+      <c r="C81" s="4" t="s">
         <v>393</v>
       </c>
-      <c t="s" s="4" r="C81">
+      <c r="D81" s="4" t="s">
         <v>394</v>
       </c>
-      <c t="s" s="4" r="D81">
+      <c r="E81" s="5"/>
+      <c r="F81" s="5"/>
+      <c r="G81" s="5"/>
+      <c r="H81" s="5"/>
+      <c r="I81" s="5"/>
+      <c r="J81" s="5"/>
+    </row>
+    <row r="82" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A82" s="4" t="s">
         <v>395</v>
       </c>
-      <c s="5" r="E81"/>
-      <c s="5" r="F81"/>
-      <c s="5" r="G81"/>
-      <c s="5" r="H81"/>
-      <c s="5" r="I81"/>
-      <c s="5" r="J81"/>
-    </row>
-    <row r="82">
-      <c t="s" s="4" r="A82">
+      <c r="B82" s="4" t="s">
         <v>396</v>
       </c>
-      <c t="s" s="4" r="B82">
+      <c r="C82" s="4" t="s">
         <v>397</v>
       </c>
-      <c t="s" s="4" r="C82">
+      <c r="D82" s="4" t="s">
         <v>398</v>
       </c>
-      <c t="s" s="4" r="D82">
+      <c r="E82" s="4" t="s">
         <v>399</v>
       </c>
-      <c t="s" s="4" r="E82">
+      <c r="F82" s="5"/>
+      <c r="G82" s="5"/>
+      <c r="H82" s="5"/>
+      <c r="I82" s="5"/>
+      <c r="J82" s="5"/>
+    </row>
+    <row r="83" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A83" s="4" t="s">
         <v>400</v>
       </c>
-      <c s="5" r="F82"/>
-      <c s="5" r="G82"/>
-      <c s="5" r="H82"/>
-      <c s="5" r="I82"/>
-      <c s="5" r="J82"/>
-    </row>
-    <row r="83">
-      <c t="s" s="4" r="A83">
+      <c r="B83" s="5"/>
+      <c r="C83" s="4" t="s">
         <v>401</v>
       </c>
-      <c s="5" r="B83"/>
-      <c t="s" s="4" r="C83">
+      <c r="D83" s="4" t="s">
         <v>402</v>
       </c>
-      <c t="s" s="4" r="D83">
+      <c r="E83" s="4" t="s">
         <v>403</v>
       </c>
-      <c t="s" s="4" r="E83">
-        <v>404</v>
-      </c>
-      <c s="5" r="F83"/>
-      <c s="5" r="G83"/>
-      <c s="5" r="H83"/>
-      <c s="5" r="I83"/>
-      <c s="5" r="J83"/>
-    </row>
-    <row r="84">
-      <c s="6" r="A84"/>
+      <c r="F83" s="5"/>
+      <c r="G83" s="5"/>
+      <c r="H83" s="5"/>
+      <c r="I83" s="5"/>
+      <c r="J83" s="5"/>
+    </row>
+    <row r="84" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A84" s="6"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink ref="H72" r:id="rId1" tooltip="2368258" display="http://es.farnell.com/texas-instruments/tps2115apwr/ic-autoswing-power-mux-5-5v-8/dp/2368258"/>
+    <hyperlink ref="I72" r:id="rId2" tooltip="94T5091" display="http://www.newark.com/texas-instruments/tps2115apwr/ic-autoswing-power-mux-5-5v-8/dp/94T5091"/>
+    <hyperlink ref="J72" r:id="rId3" display="http://www.digikey.es/product-detail/en/TPS2115APWR/296-16940-1-ND/652794"/>
+    <hyperlink ref="J73" r:id="rId4" display="http://www.digikey.es/product-detail/en/0475710001/WM9731CT-ND/4037907"/>
+    <hyperlink ref="H2" r:id="rId5" tooltip="1362417" display="http://es.farnell.com/yageo-phycomp/cc0402zry5v7bb104/cap-mlcc-y5v-100nf-16v-0402-reel/dp/1362417"/>
+    <hyperlink ref="I2" r:id="rId6" tooltip="68R4688" display="http://www.newark.com/yageo/cc0402zry5v7bb104/capacitor-ceramic-0-1uf-16v-y5v/dp/68R4688"/>
+    <hyperlink ref="J2" r:id="rId7" display="http://www.digikey.es/product-detail/en/CC0402ZRY5V7BB104/311-1047-2-ND/302781"/>
+    <hyperlink ref="H3" r:id="rId8" tooltip="1362417" display="http://es.farnell.com/yageo-phycomp/cc0402zry5v7bb104/cap-mlcc-y5v-100nf-16v-0402-reel/dp/1362417"/>
+    <hyperlink ref="I3" r:id="rId9" tooltip="68R4688" display="http://www.newark.com/yageo/cc0402zry5v7bb104/capacitor-ceramic-0-1uf-16v-y5v/dp/68R4688"/>
+    <hyperlink ref="J3" r:id="rId10" display="http://www.digikey.es/product-detail/en/CC0402ZRY5V7BB104/311-1047-2-ND/302781"/>
+    <hyperlink ref="J6" r:id="rId11" display="http://www.digikey.es/product-detail/en/CC0402ZRY5V7BB104/311-1047-2-ND/302781"/>
+    <hyperlink ref="I6" r:id="rId12" tooltip="68R4688" display="http://www.newark.com/yageo/cc0402zry5v7bb104/capacitor-ceramic-0-1uf-16v-y5v/dp/68R4688"/>
+    <hyperlink ref="H6" r:id="rId13" tooltip="1362417" display="http://es.farnell.com/yageo-phycomp/cc0402zry5v7bb104/cap-mlcc-y5v-100nf-16v-0402-reel/dp/1362417"/>
+    <hyperlink ref="H7" r:id="rId14" tooltip="1362417" display="http://es.farnell.com/yageo-phycomp/cc0402zry5v7bb104/cap-mlcc-y5v-100nf-16v-0402-reel/dp/1362417"/>
+    <hyperlink ref="I7" r:id="rId15" tooltip="68R4688" display="http://www.newark.com/yageo/cc0402zry5v7bb104/capacitor-ceramic-0-1uf-16v-y5v/dp/68R4688"/>
+    <hyperlink ref="J7" r:id="rId16" display="http://www.digikey.es/product-detail/en/CC0402ZRY5V7BB104/311-1047-2-ND/302781"/>
+    <hyperlink ref="H8" r:id="rId17" tooltip="1362417" display="http://es.farnell.com/yageo-phycomp/cc0402zry5v7bb104/cap-mlcc-y5v-100nf-16v-0402-reel/dp/1362417"/>
+    <hyperlink ref="I8" r:id="rId18" tooltip="68R4688" display="http://www.newark.com/yageo/cc0402zry5v7bb104/capacitor-ceramic-0-1uf-16v-y5v/dp/68R4688"/>
+    <hyperlink ref="J8" r:id="rId19" display="http://www.digikey.es/product-detail/en/CC0402ZRY5V7BB104/311-1047-2-ND/302781"/>
+    <hyperlink ref="H9" r:id="rId20" tooltip="1362417" display="http://es.farnell.com/yageo-phycomp/cc0402zry5v7bb104/cap-mlcc-y5v-100nf-16v-0402-reel/dp/1362417"/>
+    <hyperlink ref="I9" r:id="rId21" tooltip="68R4688" display="http://www.newark.com/yageo/cc0402zry5v7bb104/capacitor-ceramic-0-1uf-16v-y5v/dp/68R4688"/>
+    <hyperlink ref="J9" r:id="rId22" display="http://www.digikey.es/product-detail/en/CC0402ZRY5V7BB104/311-1047-2-ND/302781"/>
+    <hyperlink ref="J10" r:id="rId23" display="http://www.digikey.es/product-detail/en/CC0402ZRY5V7BB104/311-1047-2-ND/302781"/>
+    <hyperlink ref="I10" r:id="rId24" tooltip="68R4688" display="http://www.newark.com/yageo/cc0402zry5v7bb104/capacitor-ceramic-0-1uf-16v-y5v/dp/68R4688"/>
+    <hyperlink ref="H10" r:id="rId25" tooltip="1362417" display="http://es.farnell.com/yageo-phycomp/cc0402zry5v7bb104/cap-mlcc-y5v-100nf-16v-0402-reel/dp/1362417"/>
+    <hyperlink ref="H11" r:id="rId26" tooltip="1362417" display="http://es.farnell.com/yageo-phycomp/cc0402zry5v7bb104/cap-mlcc-y5v-100nf-16v-0402-reel/dp/1362417"/>
+    <hyperlink ref="I11" r:id="rId27" tooltip="68R4688" display="http://www.newark.com/yageo/cc0402zry5v7bb104/capacitor-ceramic-0-1uf-16v-y5v/dp/68R4688"/>
+    <hyperlink ref="J11" r:id="rId28" display="http://www.digikey.es/product-detail/en/CC0402ZRY5V7BB104/311-1047-2-ND/302781"/>
+    <hyperlink ref="H14" r:id="rId29" tooltip="1362417" display="http://es.farnell.com/yageo-phycomp/cc0402zry5v7bb104/cap-mlcc-y5v-100nf-16v-0402-reel/dp/1362417"/>
+    <hyperlink ref="I14" r:id="rId30" tooltip="68R4688" display="http://www.newark.com/yageo/cc0402zry5v7bb104/capacitor-ceramic-0-1uf-16v-y5v/dp/68R4688"/>
+    <hyperlink ref="J14" r:id="rId31" display="http://www.digikey.es/product-detail/en/CC0402ZRY5V7BB104/311-1047-2-ND/302781"/>
+    <hyperlink ref="H15" r:id="rId32" tooltip="1362417" display="http://es.farnell.com/yageo-phycomp/cc0402zry5v7bb104/cap-mlcc-y5v-100nf-16v-0402-reel/dp/1362417"/>
+    <hyperlink ref="I15" r:id="rId33" tooltip="68R4688" display="http://www.newark.com/yageo/cc0402zry5v7bb104/capacitor-ceramic-0-1uf-16v-y5v/dp/68R4688"/>
+    <hyperlink ref="J15" r:id="rId34" display="http://www.digikey.es/product-detail/en/CC0402ZRY5V7BB104/311-1047-2-ND/302781"/>
+    <hyperlink ref="H17" r:id="rId35" tooltip="1362417" display="http://es.farnell.com/yageo-phycomp/cc0402zry5v7bb104/cap-mlcc-y5v-100nf-16v-0402-reel/dp/1362417"/>
+    <hyperlink ref="I17" r:id="rId36" tooltip="68R4688" display="http://www.newark.com/yageo/cc0402zry5v7bb104/capacitor-ceramic-0-1uf-16v-y5v/dp/68R4688"/>
+    <hyperlink ref="J17" r:id="rId37" display="http://www.digikey.es/product-detail/en/CC0402ZRY5V7BB104/311-1047-2-ND/302781"/>
+    <hyperlink ref="H18" r:id="rId38" tooltip="1362417" display="http://es.farnell.com/yageo-phycomp/cc0402zry5v7bb104/cap-mlcc-y5v-100nf-16v-0402-reel/dp/1362417"/>
+    <hyperlink ref="I18" r:id="rId39" tooltip="68R4688" display="http://www.newark.com/yageo/cc0402zry5v7bb104/capacitor-ceramic-0-1uf-16v-y5v/dp/68R4688"/>
+    <hyperlink ref="J18" r:id="rId40" display="http://www.digikey.es/product-detail/en/CC0402ZRY5V7BB104/311-1047-2-ND/302781"/>
+    <hyperlink ref="H19" r:id="rId41" tooltip="1362417" display="http://es.farnell.com/yageo-phycomp/cc0402zry5v7bb104/cap-mlcc-y5v-100nf-16v-0402-reel/dp/1362417"/>
+    <hyperlink ref="I19" r:id="rId42" tooltip="68R4688" display="http://www.newark.com/yageo/cc0402zry5v7bb104/capacitor-ceramic-0-1uf-16v-y5v/dp/68R4688"/>
+    <hyperlink ref="J19" r:id="rId43" display="http://www.digikey.es/product-detail/en/CC0402ZRY5V7BB104/311-1047-2-ND/302781"/>
+    <hyperlink ref="J21" r:id="rId44" display="http://www.digikey.es/product-detail/en/CC0402ZRY5V7BB104/311-1047-2-ND/302781"/>
+    <hyperlink ref="I21" r:id="rId45" tooltip="68R4688" display="http://www.newark.com/yageo/cc0402zry5v7bb104/capacitor-ceramic-0-1uf-16v-y5v/dp/68R4688"/>
+    <hyperlink ref="H21" r:id="rId46" tooltip="1362417" display="http://es.farnell.com/yageo-phycomp/cc0402zry5v7bb104/cap-mlcc-y5v-100nf-16v-0402-reel/dp/1362417"/>
+    <hyperlink ref="H25" r:id="rId47" tooltip="1362417" display="http://es.farnell.com/yageo-phycomp/cc0402zry5v7bb104/cap-mlcc-y5v-100nf-16v-0402-reel/dp/1362417"/>
+    <hyperlink ref="I25" r:id="rId48" tooltip="68R4688" display="http://www.newark.com/yageo/cc0402zry5v7bb104/capacitor-ceramic-0-1uf-16v-y5v/dp/68R4688"/>
+    <hyperlink ref="J25" r:id="rId49" display="http://www.digikey.es/product-detail/en/CC0402ZRY5V7BB104/311-1047-2-ND/302781"/>
+    <hyperlink ref="J26" r:id="rId50" display="http://www.digikey.es/product-detail/en/CC0402ZRY5V7BB104/311-1047-2-ND/302781"/>
+    <hyperlink ref="I26" r:id="rId51" tooltip="68R4688" display="http://www.newark.com/yageo/cc0402zry5v7bb104/capacitor-ceramic-0-1uf-16v-y5v/dp/68R4688"/>
+    <hyperlink ref="H26" r:id="rId52" tooltip="1362417" display="http://es.farnell.com/yageo-phycomp/cc0402zry5v7bb104/cap-mlcc-y5v-100nf-16v-0402-reel/dp/1362417"/>
+    <hyperlink ref="H27" r:id="rId53" tooltip="1362417" display="http://es.farnell.com/yageo-phycomp/cc0402zry5v7bb104/cap-mlcc-y5v-100nf-16v-0402-reel/dp/1362417"/>
+    <hyperlink ref="I27" r:id="rId54" tooltip="68R4688" display="http://www.newark.com/yageo/cc0402zry5v7bb104/capacitor-ceramic-0-1uf-16v-y5v/dp/68R4688"/>
+    <hyperlink ref="J27" r:id="rId55" display="http://www.digikey.es/product-detail/en/CC0402ZRY5V7BB104/311-1047-2-ND/302781"/>
+    <hyperlink ref="J28" r:id="rId56" display="http://www.digikey.es/product-detail/en/CC0402ZRY5V7BB104/311-1047-2-ND/302781"/>
+    <hyperlink ref="I28" r:id="rId57" tooltip="68R4688" display="http://www.newark.com/yageo/cc0402zry5v7bb104/capacitor-ceramic-0-1uf-16v-y5v/dp/68R4688"/>
+    <hyperlink ref="H28" r:id="rId58" tooltip="1362417" display="http://es.farnell.com/yageo-phycomp/cc0402zry5v7bb104/cap-mlcc-y5v-100nf-16v-0402-reel/dp/1362417"/>
+    <hyperlink ref="H29" r:id="rId59" tooltip="1362417" display="http://es.farnell.com/yageo-phycomp/cc0402zry5v7bb104/cap-mlcc-y5v-100nf-16v-0402-reel/dp/1362417"/>
+    <hyperlink ref="I29" r:id="rId60" tooltip="68R4688" display="http://www.newark.com/yageo/cc0402zry5v7bb104/capacitor-ceramic-0-1uf-16v-y5v/dp/68R4688"/>
+    <hyperlink ref="J29" r:id="rId61" display="http://www.digikey.es/product-detail/en/CC0402ZRY5V7BB104/311-1047-2-ND/302781"/>
+    <hyperlink ref="H31" r:id="rId62" tooltip="1362417" display="http://es.farnell.com/yageo-phycomp/cc0402zry5v7bb104/cap-mlcc-y5v-100nf-16v-0402-reel/dp/1362417"/>
+    <hyperlink ref="I31" r:id="rId63" tooltip="68R4688" display="http://www.newark.com/yageo/cc0402zry5v7bb104/capacitor-ceramic-0-1uf-16v-y5v/dp/68R4688"/>
+    <hyperlink ref="J31" r:id="rId64" display="http://www.digikey.es/product-detail/en/CC0402ZRY5V7BB104/311-1047-2-ND/302781"/>
+    <hyperlink ref="J32" r:id="rId65" display="http://www.digikey.es/product-detail/en/CC0402ZRY5V7BB104/311-1047-2-ND/302781"/>
+    <hyperlink ref="I32" r:id="rId66" tooltip="68R4688" display="http://www.newark.com/yageo/cc0402zry5v7bb104/capacitor-ceramic-0-1uf-16v-y5v/dp/68R4688"/>
+    <hyperlink ref="H32" r:id="rId67" tooltip="1362417" display="http://es.farnell.com/yageo-phycomp/cc0402zry5v7bb104/cap-mlcc-y5v-100nf-16v-0402-reel/dp/1362417"/>
+    <hyperlink ref="H35" r:id="rId68" tooltip="1362417" display="http://es.farnell.com/yageo-phycomp/cc0402zry5v7bb104/cap-mlcc-y5v-100nf-16v-0402-reel/dp/1362417"/>
+    <hyperlink ref="I35" r:id="rId69" tooltip="68R4688" display="http://www.newark.com/yageo/cc0402zry5v7bb104/capacitor-ceramic-0-1uf-16v-y5v/dp/68R4688"/>
+    <hyperlink ref="J35" r:id="rId70" display="http://www.digikey.es/product-detail/en/CC0402ZRY5V7BB104/311-1047-2-ND/302781"/>
+    <hyperlink ref="J36" r:id="rId71" display="http://www.digikey.es/product-detail/en/CC0402ZRY5V7BB104/311-1047-2-ND/302781"/>
+    <hyperlink ref="I36" r:id="rId72" tooltip="68R4688" display="http://www.newark.com/yageo/cc0402zry5v7bb104/capacitor-ceramic-0-1uf-16v-y5v/dp/68R4688"/>
+    <hyperlink ref="H36" r:id="rId73" tooltip="1362417" display="http://es.farnell.com/yageo-phycomp/cc0402zry5v7bb104/cap-mlcc-y5v-100nf-16v-0402-reel/dp/1362417"/>
+    <hyperlink ref="H37" r:id="rId74" tooltip="1362417" display="http://es.farnell.com/yageo-phycomp/cc0402zry5v7bb104/cap-mlcc-y5v-100nf-16v-0402-reel/dp/1362417"/>
+    <hyperlink ref="I37" r:id="rId75" tooltip="68R4688" display="http://www.newark.com/yageo/cc0402zry5v7bb104/capacitor-ceramic-0-1uf-16v-y5v/dp/68R4688"/>
+    <hyperlink ref="J37" r:id="rId76" display="http://www.digikey.es/product-detail/en/CC0402ZRY5V7BB104/311-1047-2-ND/302781"/>
+    <hyperlink ref="H41" r:id="rId77" tooltip="1362417" display="http://es.farnell.com/yageo-phycomp/cc0402zry5v7bb104/cap-mlcc-y5v-100nf-16v-0402-reel/dp/1362417"/>
+    <hyperlink ref="I41" r:id="rId78" tooltip="68R4688" display="http://www.newark.com/yageo/cc0402zry5v7bb104/capacitor-ceramic-0-1uf-16v-y5v/dp/68R4688"/>
+    <hyperlink ref="J41" r:id="rId79" display="http://www.digikey.es/product-detail/en/CC0402ZRY5V7BB104/311-1047-2-ND/302781"/>
+    <hyperlink ref="H4" r:id="rId80" tooltip="2390053" display="http://es.farnell.com/kemet/t527i476m010ate200/cap-tant-47uf-10v-case-i/dp/2390053"/>
+    <hyperlink ref="J4" r:id="rId81" display="http://www.digikey.es/product-detail/en/T527I476M010ATE200/399-10532-1-ND/4246291"/>
+    <hyperlink ref="H5" r:id="rId82" tooltip="2346884" display="http://es.farnell.com/tdk/c1005x5r1e105k050bc/cap-mlcc-x5r-1uf-25v-0402/dp/2346884"/>
+    <hyperlink ref="I5" r:id="rId83" tooltip="05X9838" display="http://www.newark.com/tdk/c1005x5r1e105k050bc/cap-mlcc-x5r-1uf-25v-0402/dp/05X9838"/>
+    <hyperlink ref="J5" r:id="rId84" display="http://www.digikey.es/product-detail/en/C1005X5R1E105K050BC/445-9066-1-ND/3648637"/>
+    <hyperlink ref="J12" r:id="rId85" display="http://www.digikey.es/product-detail/en/F931A107KBA/478-8195-2-ND/4005266"/>
+    <hyperlink ref="H13" r:id="rId86" tooltip="2425585" display="http://es.farnell.com/vishay/tl8a0107m010c/cap-tant-100uf-10v-case-a0/dp/2425585"/>
+    <hyperlink ref="J13" r:id="rId87" display="http://www.digikey.es/product-detail/en/TL8A0107M010C/718-1921-1-ND/3883166"/>
+    <hyperlink ref="H16" r:id="rId88" tooltip="2346881" display="http://es.farnell.com/tdk/c1005x5r1a475m050bc/cap-mlcc-x5r-4-7uf-10v-0402/dp/2346881"/>
+    <hyperlink ref="I16" r:id="rId89" tooltip="04X3214" display="http://www.newark.com/tdk/c1005x5r1a475m050bc/cap-ceramic-4-7uf-10v-x5r-0402/dp/04X3214"/>
+    <hyperlink ref="J16" r:id="rId90" display="http://www.digikey.es/product-detail/en/C1005X5R1A475M050BC/445-8023-1-ND/2792141"/>
+    <hyperlink ref="H20" r:id="rId91" tooltip="2346881" display="http://es.farnell.com/tdk/c1005x5r1a475m050bc/cap-mlcc-x5r-4-7uf-10v-0402/dp/2346881"/>
+    <hyperlink ref="I20" r:id="rId92" tooltip="04X3214" display="http://www.newark.com/tdk/c1005x5r1a475m050bc/cap-ceramic-4-7uf-10v-x5r-0402/dp/04X3214"/>
+    <hyperlink ref="J20" r:id="rId93" display="http://www.digikey.es/product-detail/en/C1005X5R1A475M050BC/445-8023-1-ND/2792141"/>
+    <hyperlink ref="H22" r:id="rId94" tooltip="2425585" display="http://es.farnell.com/vishay/tl8a0107m010c/cap-tant-100uf-10v-case-a0/dp/2425585"/>
+    <hyperlink ref="J22" r:id="rId95" display="http://www.digikey.es/product-detail/en/TL8A0107M010C/718-1921-1-ND/3883166"/>
+    <hyperlink ref="J23" r:id="rId96" display="http://www.digikey.es/product-detail/en/C1005X5R0J106M050BC/445-8920-1-ND/3507812"/>
+    <hyperlink ref="H23" r:id="rId97" tooltip="2346872" display="http://es.farnell.com/tdk/c1005x5r0j106m050bc/cap-mlcc-x5r-10uf-6-3v-0402/dp/2346872"/>
+    <hyperlink ref="H24" r:id="rId98" tooltip="2346872" display="http://es.farnell.com/tdk/c1005x5r0j106m050bc/cap-mlcc-x5r-10uf-6-3v-0402/dp/2346872"/>
+    <hyperlink ref="J24" r:id="rId99" display="http://www.digikey.es/product-detail/en/C1005X5R0J106M050BC/445-8920-1-ND/3507812"/>
+    <hyperlink ref="H30" r:id="rId100" tooltip="2426961" display="http://es.farnell.com/murata/grm219r61e106ka12d/cap-mlcc-x5r-10uf-25v-0805/dp/2426961"/>
+    <hyperlink ref="J30" r:id="rId101" display="http://www.digikey.es/product-detail/en/GRM219R61E106KA12D/490-7207-1-ND/3900481"/>
+    <hyperlink ref="J33" r:id="rId102" display="http://www.digikey.es/product-detail/en/C1005X5R1A225K050BC/445-7392-1-ND/2733464"/>
+    <hyperlink ref="H33" r:id="rId103" tooltip="2346879" display="http://es.farnell.com/tdk/c1005x5r1a225k050bc/cap-mlcc-x5r-2-2uf-10v-0402/dp/2346879"/>
+    <hyperlink ref="I33" r:id="rId104" tooltip="04X3212" display="http://www.newark.com/tdk/c1005x5r1a225k050bc/cap-ceramic-2-2uf-10v-x5r-0402/dp/04X3212"/>
+    <hyperlink ref="H34" r:id="rId105" tooltip="2346879" display="http://es.farnell.com/tdk/c1005x5r1a225k050bc/cap-mlcc-x5r-2-2uf-10v-0402/dp/2346879"/>
+    <hyperlink ref="I34" r:id="rId106" tooltip="04X3212" display="http://www.newark.com/tdk/c1005x5r1a225k050bc/cap-ceramic-2-2uf-10v-x5r-0402/dp/04X3212"/>
+    <hyperlink ref="J34" r:id="rId107" display="http://www.digikey.es/product-detail/en/C1005X5R1A225K050BC/445-7392-1-ND/2733464"/>
+    <hyperlink ref="H38" r:id="rId108" tooltip="1658510" display="http://es.farnell.com/avx/tpsb107m010r0400/cap-tant-100uf-10v-case-b/dp/1658510"/>
+    <hyperlink ref="J38" r:id="rId109" display="http://www.digikey.es/product-detail/en/TPSB107M010R0400/478-5231-2-ND/1472679"/>
+    <hyperlink ref="I38" r:id="rId110" tooltip="10R5878" display="http://www.newark.com/avx/tpsb107m010r0400/capacitor-tant-100uf-10v-0-4-ohm/dp/10R5878"/>
+    <hyperlink ref="J39" r:id="rId111" display="http://www.digikey.es/product-detail/en/500R07S180GV4T/712-1264-1-ND/1786726"/>
+    <hyperlink ref="I39" r:id="rId112" tooltip="41M1570" display="http://www.newark.com/johanson-technology/500r07s180gv4t/capacitor-rf-ceramic-18pf-50v/dp/41M1570"/>
+    <hyperlink ref="H39" r:id="rId113" tooltip="1650783" display="http://es.farnell.com/johanson-technology/500r07s180gv4t/capacitor-ceramic-multilayer/dp/1650783"/>
+    <hyperlink ref="H40" r:id="rId114" tooltip="1650783" display="http://es.farnell.com/johanson-technology/500r07s180gv4t/capacitor-ceramic-multilayer/dp/1650783"/>
+    <hyperlink ref="I40" r:id="rId115" tooltip="41M1570" display="http://www.newark.com/johanson-technology/500r07s180gv4t/capacitor-rf-ceramic-18pf-50v/dp/41M1570"/>
+    <hyperlink ref="J40" r:id="rId116" display="http://www.digikey.es/product-detail/en/500R07S180GV4T/712-1264-1-ND/1786726"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId117"/>
 </worksheet>
 </file>
</xml_diff>